<commit_message>
Re-organize codes to protect reproducibility of variables EDA part.
</commit_message>
<xml_diff>
--- a/Data/cleaned/Manufacturing_filled.xlsx
+++ b/Data/cleaned/Manufacturing_filled.xlsx
@@ -11148,7 +11148,7 @@
         <v>1080060319096.752</v>
       </c>
       <c r="M2">
-        <v>6.652950196607194</v>
+        <v>6.652950196607193</v>
       </c>
       <c r="N2">
         <v>31.97506997026333</v>
@@ -11192,7 +11192,7 @@
         <v>1243212055648.438</v>
       </c>
       <c r="M3">
-        <v>6.652950196607194</v>
+        <v>6.652950196607193</v>
       </c>
       <c r="N3">
         <v>32.09392432867769</v>
@@ -11236,7 +11236,7 @@
         <v>1446864352020.468</v>
       </c>
       <c r="M4">
-        <v>6.652950196607194</v>
+        <v>6.652950196607193</v>
       </c>
       <c r="N4">
         <v>32.45232805659434</v>
@@ -11280,7 +11280,7 @@
         <v>1810542998093.986</v>
       </c>
       <c r="M5">
-        <v>6.652950196607194</v>
+        <v>6.652950196607193</v>
       </c>
       <c r="N5">
         <v>32.38335311644068</v>
@@ -11324,7 +11324,7 @@
         <v>2286747160116.281</v>
       </c>
       <c r="M6">
-        <v>6.652950196607194</v>
+        <v>6.652950196607193</v>
       </c>
       <c r="N6">
         <v>32.11941160334752</v>
@@ -11368,7 +11368,7 @@
         <v>2554946777468.748</v>
       </c>
       <c r="M7">
-        <v>6.652950196607194</v>
+        <v>6.652950196607193</v>
       </c>
       <c r="N7">
         <v>31.59623809103104</v>
@@ -11875,7 +11875,7 @@
         <v>69.99140475588121</v>
       </c>
       <c r="F19">
-        <v>143.8155463696435</v>
+        <v>143.8155463696434</v>
       </c>
       <c r="G19">
         <v>2.894901043785465</v>
@@ -11896,7 +11896,7 @@
         <v>4393454792660.693</v>
       </c>
       <c r="M19">
-        <v>6.652950196607194</v>
+        <v>6.652950196607193</v>
       </c>
       <c r="N19">
         <v>27.43772961721378</v>
@@ -16993,7 +16993,7 @@
         <v>33.50310345353751</v>
       </c>
       <c r="C2">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D2">
         <v>3770.548034667971</v>
@@ -17037,7 +17037,7 @@
         <v>41.3400001525879</v>
       </c>
       <c r="C3">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D3">
         <v>3770.548034667971</v>
@@ -17081,7 +17081,7 @@
         <v>41</v>
       </c>
       <c r="C4">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D4">
         <v>3770.548034667971</v>
@@ -17125,7 +17125,7 @@
         <v>40.6599998474121</v>
       </c>
       <c r="C5">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D5">
         <v>3770.548034667971</v>
@@ -17169,7 +17169,7 @@
         <v>38.939998626709</v>
       </c>
       <c r="C6">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D6">
         <v>3770.548034667971</v>
@@ -17213,7 +17213,7 @@
         <v>38.4000015258789</v>
       </c>
       <c r="C7">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D7">
         <v>3770.548034667971</v>
@@ -18313,7 +18313,7 @@
         <v>33.50310345353751</v>
       </c>
       <c r="C32">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D32">
         <v>3770.548034667971</v>
@@ -18357,7 +18357,7 @@
         <v>33.50310345353751</v>
       </c>
       <c r="C33">
-        <v>1.610600824157397</v>
+        <v>1.610600824157396</v>
       </c>
       <c r="D33">
         <v>3770.548034667971</v>
@@ -18372,7 +18372,7 @@
         <v>3.812286684094758</v>
       </c>
       <c r="H33">
-        <v>5637.119960567888</v>
+        <v>5637.119960567889</v>
       </c>
       <c r="I33">
         <v>8492100.326052006</v>
@@ -26295,7 +26295,7 @@
         <v>0.9587291335344367</v>
       </c>
       <c r="H43">
-        <v>942.1436104697207</v>
+        <v>942.1436104697204</v>
       </c>
       <c r="I43">
         <v>9111306.96190476</v>
@@ -32969,7 +32969,7 @@
         <v>3373095791123.574</v>
       </c>
       <c r="M2">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N2">
         <v>23.46921539563932</v>
@@ -33013,7 +33013,7 @@
         <v>3761198219001.569</v>
       </c>
       <c r="M3">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N3">
         <v>23.47176597231475</v>
@@ -33057,7 +33057,7 @@
         <v>3327988556625.308</v>
       </c>
       <c r="M4">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N4">
         <v>23.36115643732072</v>
@@ -33101,7 +33101,7 @@
         <v>3050631080519.279</v>
       </c>
       <c r="M5">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N5">
         <v>23.35048737419174</v>
@@ -33145,7 +33145,7 @@
         <v>2814130520307.428</v>
       </c>
       <c r="M6">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N6">
         <v>22.83664375633507</v>
@@ -33189,7 +33189,7 @@
         <v>3259750076378.232</v>
       </c>
       <c r="M7">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N7">
         <v>22.40186384416154</v>
@@ -33233,7 +33233,7 @@
         <v>3488679586695.185</v>
       </c>
       <c r="M8">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N8">
         <v>22.45220880818845</v>
@@ -33277,7 +33277,7 @@
         <v>3134526849169.21</v>
       </c>
       <c r="M9">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N9">
         <v>21.11971716938407</v>
@@ -33321,7 +33321,7 @@
         <v>3046675120426.197</v>
       </c>
       <c r="M10">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N10">
         <v>20.71470204605068</v>
@@ -33365,7 +33365,7 @@
         <v>3287238805004.593</v>
       </c>
       <c r="M11">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N11">
         <v>20.91713129374546</v>
@@ -33409,7 +33409,7 @@
         <v>3545239525662.474</v>
       </c>
       <c r="M12">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N12">
         <v>21.12059121924424</v>
@@ -33453,7 +33453,7 @@
         <v>3505028207682.579</v>
       </c>
       <c r="M13">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N13">
         <v>21.42337238571039</v>
@@ -33497,7 +33497,7 @@
         <v>3341916073441.542</v>
       </c>
       <c r="M14">
-        <v>0.2283290883278704</v>
+        <v>0.2283290883278703</v>
       </c>
       <c r="N14">
         <v>21.3992856851895</v>
@@ -34080,7 +34080,7 @@
         <v>2020</v>
       </c>
       <c r="B28">
-        <v>35.48961522028996</v>
+        <v>35.48961522028997</v>
       </c>
       <c r="C28">
         <v>3.26317000389099</v>
@@ -39990,7 +39990,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C2">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D2">
         <v>5422.810414632161</v>
@@ -40020,7 +40020,7 @@
         <v>7155338912.903522</v>
       </c>
       <c r="M2">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N2">
         <v>26.52611559513869</v>
@@ -40034,7 +40034,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C3">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D3">
         <v>5422.810414632161</v>
@@ -40064,7 +40064,7 @@
         <v>8124089295.722025</v>
       </c>
       <c r="M3">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N3">
         <v>25.7581049024776</v>
@@ -40078,7 +40078,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C4">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D4">
         <v>5422.810414632161</v>
@@ -40108,7 +40108,7 @@
         <v>9082027737.018982</v>
       </c>
       <c r="M4">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N4">
         <v>22.29291490588914</v>
@@ -40122,7 +40122,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C5">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D5">
         <v>5422.810414632161</v>
@@ -40152,7 +40152,7 @@
         <v>9679906542.056074</v>
       </c>
       <c r="M5">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N5">
         <v>21.46434389615849</v>
@@ -40166,7 +40166,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C6">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D6">
         <v>5422.810414632161</v>
@@ -40196,7 +40196,7 @@
         <v>10693942262.18646</v>
       </c>
       <c r="M6">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N6">
         <v>21.40238291509307</v>
@@ -40210,7 +40210,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C7">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D7">
         <v>5422.810414632161</v>
@@ -40240,7 +40240,7 @@
         <v>11138812057.5688</v>
       </c>
       <c r="M7">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N7">
         <v>20.11536164922619</v>
@@ -40254,7 +40254,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C8">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D8">
         <v>5422.810414632161</v>
@@ -40284,7 +40284,7 @@
         <v>11013181219.0355</v>
       </c>
       <c r="M8">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N8">
         <v>22.61381615789615</v>
@@ -40298,7 +40298,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C9">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D9">
         <v>5422.810414632161</v>
@@ -40328,7 +40328,7 @@
         <v>12267704601.81868</v>
       </c>
       <c r="M9">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N9">
         <v>24.09005587328071</v>
@@ -40342,7 +40342,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C10">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D10">
         <v>5422.810414632161</v>
@@ -40372,7 +40372,7 @@
         <v>14288888888.88889</v>
       </c>
       <c r="M10">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N10">
         <v>26.07842073053191</v>
@@ -40386,7 +40386,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C11">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D11">
         <v>5422.810414632161</v>
@@ -40416,7 +40416,7 @@
         <v>16926505664.87776</v>
       </c>
       <c r="M11">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N11">
         <v>25.30122250585156</v>
@@ -40430,7 +40430,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C12">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D12">
         <v>5422.810414632161</v>
@@ -40460,7 +40460,7 @@
         <v>19552222734.96385</v>
       </c>
       <c r="M12">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N12">
         <v>24.40422570975837</v>
@@ -40474,7 +40474,7 @@
         <v>36.560001373291</v>
       </c>
       <c r="C13">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D13">
         <v>5422.810414632161</v>
@@ -40504,7 +40504,7 @@
         <v>23865354558.61071</v>
       </c>
       <c r="M13">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N13">
         <v>25.45987665323874</v>
@@ -40518,7 +40518,7 @@
         <v>36.189998626709</v>
       </c>
       <c r="C14">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D14">
         <v>5422.810414632161</v>
@@ -40548,7 +40548,7 @@
         <v>27188643339.47207</v>
       </c>
       <c r="M14">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N14">
         <v>24.34968358529537</v>
@@ -40562,7 +40562,7 @@
         <v>36.0699996948242</v>
       </c>
       <c r="C15">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D15">
         <v>5422.810414632161</v>
@@ -40592,7 +40592,7 @@
         <v>31898811734.12551</v>
       </c>
       <c r="M15">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N15">
         <v>24.47185597678178</v>
@@ -40606,7 +40606,7 @@
         <v>35.4199981689453</v>
       </c>
       <c r="C16">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D16">
         <v>5422.810414632161</v>
@@ -40636,7 +40636,7 @@
         <v>37684758412.9894</v>
       </c>
       <c r="M16">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N16">
         <v>23.62472169260649</v>
@@ -40650,7 +40650,7 @@
         <v>34.6699981689453</v>
       </c>
       <c r="C17">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D17">
         <v>5422.810414632161</v>
@@ -40680,7 +40680,7 @@
         <v>43132707774.79893</v>
       </c>
       <c r="M17">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N17">
         <v>23.98506226333385</v>
@@ -40724,7 +40724,7 @@
         <v>47546595744.68085</v>
       </c>
       <c r="M18">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N18">
         <v>23.16721806017505</v>
@@ -40768,7 +40768,7 @@
         <v>48600282866.37931</v>
       </c>
       <c r="M19">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N19">
         <v>22.15150365521268</v>
@@ -40812,7 +40812,7 @@
         <v>41960623804.97132</v>
       </c>
       <c r="M20">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N20">
         <v>22.68745264851204</v>
@@ -40856,7 +40856,7 @@
         <v>44252330383.48083</v>
       </c>
       <c r="M21">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N21">
         <v>22.85068631305447</v>
@@ -40900,7 +40900,7 @@
         <v>50304002320.18562</v>
       </c>
       <c r="M22">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N22">
         <v>25.8614860377559</v>
@@ -40944,7 +40944,7 @@
         <v>51950773008.87425</v>
       </c>
       <c r="M23">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N23">
         <v>23.39469784741456</v>
@@ -40988,7 +40988,7 @@
         <v>53693007930.3027</v>
       </c>
       <c r="M24">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N24">
         <v>24.73764032297293</v>
@@ -41032,7 +41032,7 @@
         <v>55608540925.26691</v>
       </c>
       <c r="M25">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N25">
         <v>24.76541269319689</v>
@@ -41076,7 +41076,7 @@
         <v>60183232753.52029</v>
       </c>
       <c r="M26">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N26">
         <v>27.11936759706429</v>
@@ -41120,7 +41120,7 @@
         <v>63577925979.33189</v>
       </c>
       <c r="M27">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N27">
         <v>27.07676179820706</v>
@@ -41750,7 +41750,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C42">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D42">
         <v>5422.810414632161</v>
@@ -41794,7 +41794,7 @@
         <v>28.13827573842016</v>
       </c>
       <c r="C43">
-        <v>1.97105332215627</v>
+        <v>1.971053322156271</v>
       </c>
       <c r="D43">
         <v>5422.810414632161</v>
@@ -41824,7 +41824,7 @@
         <v>168800000000</v>
       </c>
       <c r="M43">
-        <v>7.912250304722815</v>
+        <v>7.912250304722816</v>
       </c>
       <c r="N43">
         <v>21.07415385601889</v>
@@ -49396,7 +49396,7 @@
         <v>3.45018005371094</v>
       </c>
       <c r="D25">
-        <v>3936.797055451768</v>
+        <v>3936.797055451767</v>
       </c>
       <c r="E25">
         <v>64.9973268643096</v>
@@ -56243,7 +56243,7 @@
         <v>1980</v>
       </c>
       <c r="B2">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C2">
         <v>1.122195997834206</v>
@@ -56287,7 +56287,7 @@
         <v>1981</v>
       </c>
       <c r="B3">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C3">
         <v>1.122195997834206</v>
@@ -56331,7 +56331,7 @@
         <v>1982</v>
       </c>
       <c r="B4">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C4">
         <v>1.122195997834206</v>
@@ -56375,7 +56375,7 @@
         <v>1983</v>
       </c>
       <c r="B5">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C5">
         <v>1.122195997834206</v>
@@ -56419,7 +56419,7 @@
         <v>1984</v>
       </c>
       <c r="B6">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C6">
         <v>1.122195997834206</v>
@@ -56463,7 +56463,7 @@
         <v>1985</v>
       </c>
       <c r="B7">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C7">
         <v>1.122195997834206</v>
@@ -56507,7 +56507,7 @@
         <v>1986</v>
       </c>
       <c r="B8">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C8">
         <v>1.122195997834206</v>
@@ -56551,7 +56551,7 @@
         <v>1987</v>
       </c>
       <c r="B9">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C9">
         <v>1.122195997834206</v>
@@ -56595,7 +56595,7 @@
         <v>1988</v>
       </c>
       <c r="B10">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C10">
         <v>1.122195997834206</v>
@@ -56639,7 +56639,7 @@
         <v>1989</v>
       </c>
       <c r="B11">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C11">
         <v>1.122195997834206</v>
@@ -56683,7 +56683,7 @@
         <v>1990</v>
       </c>
       <c r="B12">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C12">
         <v>1.122195997834206</v>
@@ -58003,7 +58003,7 @@
         <v>2020</v>
       </c>
       <c r="B42">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C42">
         <v>1.122195997834206</v>
@@ -58047,7 +58047,7 @@
         <v>2021</v>
       </c>
       <c r="B43">
-        <v>28.28000009470973</v>
+        <v>28.28000009470972</v>
       </c>
       <c r="C43">
         <v>1.122195997834206</v>
@@ -58062,7 +58062,7 @@
         <v>20.54229020320603</v>
       </c>
       <c r="G43">
-        <v>2.19214940663726</v>
+        <v>2.192149406637261</v>
       </c>
       <c r="H43">
         <v>1338.945431054144</v>

</xml_diff>

<commit_message>
update with imputation till 2021
</commit_message>
<xml_diff>
--- a/Data/cleaned/Manufacturing_filled.xlsx
+++ b/Data/cleaned/Manufacturing_filled.xlsx
@@ -461,7 +461,7 @@
         <v>1990</v>
       </c>
       <c r="B2">
-        <v>66.8518331046956</v>
+        <v>66.85183310469561</v>
       </c>
       <c r="C2">
         <v>2.221352980227276</v>
@@ -473,7 +473,7 @@
         <v>1222.3000488281</v>
       </c>
       <c r="F2">
-        <v>89613697575.99075</v>
+        <v>89613697575.99077</v>
       </c>
       <c r="G2">
         <v>18243.47141836716</v>
@@ -490,10 +490,10 @@
         <v>1991</v>
       </c>
       <c r="B3">
-        <v>66.85632700506464</v>
+        <v>66.85632700506466</v>
       </c>
       <c r="C3">
-        <v>2.236429208156425</v>
+        <v>2.236429208156426</v>
       </c>
       <c r="D3">
         <v>1.703353971064451</v>
@@ -519,7 +519,7 @@
         <v>1992</v>
       </c>
       <c r="B4">
-        <v>66.8282908743771</v>
+        <v>66.82829087437712</v>
       </c>
       <c r="C4">
         <v>2.251672329507407</v>
@@ -531,7 +531,7 @@
         <v>1274.299186066213</v>
       </c>
       <c r="F4">
-        <v>88979505692.53592</v>
+        <v>88979505692.53593</v>
       </c>
       <c r="G4">
         <v>18581.13797295549</v>
@@ -551,7 +551,7 @@
         <v>66.77937198644234</v>
       </c>
       <c r="C5">
-        <v>2.26585260829132</v>
+        <v>2.265852608291321</v>
       </c>
       <c r="D5">
         <v>1.654344442600021</v>
@@ -560,7 +560,7 @@
         <v>1348.552430615375</v>
       </c>
       <c r="F5">
-        <v>87427038349.29124</v>
+        <v>87427038349.29123</v>
       </c>
       <c r="G5">
         <v>18311.30264535949</v>
@@ -577,10 +577,10 @@
         <v>1994</v>
       </c>
       <c r="B6">
-        <v>66.73025807989745</v>
+        <v>66.73025807989744</v>
       </c>
       <c r="C6">
-        <v>2.280380262183471</v>
+        <v>2.28038026218347</v>
       </c>
       <c r="D6">
         <v>1.586294748374877</v>
@@ -589,7 +589,7 @@
         <v>1422.521344496953</v>
       </c>
       <c r="F6">
-        <v>87183061650.44868</v>
+        <v>87183061650.44867</v>
       </c>
       <c r="G6">
         <v>18253.53132583263</v>
@@ -624,7 +624,7 @@
         <v>18713.808884491</v>
       </c>
       <c r="H7">
-        <v>251065172786.0355</v>
+        <v>251065172786.0354</v>
       </c>
       <c r="I7">
         <v>13.12367686560688</v>
@@ -664,7 +664,7 @@
         <v>1997</v>
       </c>
       <c r="B9">
-        <v>66.65546252228495</v>
+        <v>66.65546252228496</v>
       </c>
       <c r="C9">
         <v>2.33096500288477</v>
@@ -676,7 +676,7 @@
         <v>1630.555146362744</v>
       </c>
       <c r="F9">
-        <v>95471133396.53795</v>
+        <v>95471133396.53796</v>
       </c>
       <c r="G9">
         <v>20098.94685659888</v>
@@ -696,7 +696,7 @@
         <v>66.65900548147526</v>
       </c>
       <c r="C10">
-        <v>2.348681960737215</v>
+        <v>2.348681960737216</v>
       </c>
       <c r="D10">
         <v>1.861734243325946</v>
@@ -705,7 +705,7 @@
         <v>1676.923550142231</v>
       </c>
       <c r="F10">
-        <v>96469170846.85892</v>
+        <v>96469170846.85893</v>
       </c>
       <c r="G10">
         <v>20310.09748613026</v>
@@ -722,7 +722,7 @@
         <v>1999</v>
       </c>
       <c r="B11">
-        <v>66.67326162169317</v>
+        <v>66.67326162169319</v>
       </c>
       <c r="C11">
         <v>2.367048226173048</v>
@@ -734,7 +734,7 @@
         <v>1679.49323000426</v>
       </c>
       <c r="F11">
-        <v>96369457587.53809</v>
+        <v>96369457587.5381</v>
       </c>
       <c r="G11">
         <v>20349.87604604138</v>
@@ -763,7 +763,7 @@
         <v>1687.294932047897</v>
       </c>
       <c r="F12">
-        <v>97255925118.16698</v>
+        <v>97255925118.16696</v>
       </c>
       <c r="G12">
         <v>20555.08728393575</v>
@@ -809,7 +809,7 @@
         <v>2002</v>
       </c>
       <c r="B14">
-        <v>66.77153366691425</v>
+        <v>66.77153366691427</v>
       </c>
       <c r="C14">
         <v>2.428122476147466</v>
@@ -856,7 +856,7 @@
         <v>20792.22443180106</v>
       </c>
       <c r="H15">
-        <v>297530316427.5237</v>
+        <v>297530316427.5236</v>
       </c>
       <c r="I15">
         <v>10.86216994180758</v>
@@ -899,10 +899,10 @@
         <v>66.93642093190243</v>
       </c>
       <c r="C17">
-        <v>2.496520594242284</v>
+        <v>2.496520594242285</v>
       </c>
       <c r="D17">
-        <v>2.039096983610328</v>
+        <v>2.039096983610329</v>
       </c>
       <c r="E17">
         <v>1762.230015062404</v>
@@ -911,10 +911,10 @@
         <v>113268780549.3444</v>
       </c>
       <c r="G17">
-        <v>23648.3523263318</v>
+        <v>23648.35232633181</v>
       </c>
       <c r="H17">
-        <v>346189191222.9337</v>
+        <v>346189191222.9338</v>
       </c>
       <c r="I17">
         <v>10.33486230097914</v>
@@ -946,7 +946,7 @@
         <v>372904216625.2144</v>
       </c>
       <c r="I18">
-        <v>9.892071199355792</v>
+        <v>9.892071199355795</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -975,7 +975,7 @@
         <v>405498000435.4818</v>
       </c>
       <c r="I19">
-        <v>9.290666490144647</v>
+        <v>9.290666490144645</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -986,7 +986,7 @@
         <v>67.15703304894828</v>
       </c>
       <c r="C20">
-        <v>2.572723273760545</v>
+        <v>2.572723273760546</v>
       </c>
       <c r="D20">
         <v>2.863983957741723</v>
@@ -1004,7 +1004,7 @@
         <v>451743322054.3006</v>
       </c>
       <c r="I20">
-        <v>9.202198922938425</v>
+        <v>9.202198922938424</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1059,10 +1059,10 @@
         <v>34019.70885512567</v>
       </c>
       <c r="H22">
-        <v>523290420993.8919</v>
+        <v>523290420993.892</v>
       </c>
       <c r="I22">
-        <v>7.997034212477491</v>
+        <v>7.99703421247749</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1091,7 +1091,7 @@
         <v>581701883844.9614</v>
       </c>
       <c r="I23">
-        <v>7.368513108841397</v>
+        <v>7.368513108841396</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1099,13 +1099,13 @@
         <v>2012</v>
       </c>
       <c r="B24">
-        <v>67.25040844579362</v>
+        <v>67.25040844579364</v>
       </c>
       <c r="C24">
-        <v>2.702095352144344</v>
+        <v>2.702095352144343</v>
       </c>
       <c r="D24">
-        <v>3.195082731139377</v>
+        <v>3.195082731139376</v>
       </c>
       <c r="E24">
         <v>2303.917687255045</v>
@@ -1120,7 +1120,7 @@
         <v>645302601078.7561</v>
       </c>
       <c r="I24">
-        <v>7.05045459273345</v>
+        <v>7.050454592733451</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1149,7 +1149,7 @@
         <v>705284957735.4385</v>
       </c>
       <c r="I25">
-        <v>6.608333214010963</v>
+        <v>6.608333214010962</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1163,7 +1163,7 @@
         <v>2.775172118788485</v>
       </c>
       <c r="D26">
-        <v>3.351321270008168</v>
+        <v>3.351321270008167</v>
       </c>
       <c r="E26">
         <v>2226.887369623076</v>
@@ -1172,13 +1172,13 @@
         <v>261376813478.136</v>
       </c>
       <c r="G26">
-        <v>46342.33514786843</v>
+        <v>46342.33514786842</v>
       </c>
       <c r="H26">
-        <v>748783198159.8167</v>
+        <v>748783198159.8165</v>
       </c>
       <c r="I26">
-        <v>6.368634633947076</v>
+        <v>6.368634633947077</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1198,16 +1198,16 @@
         <v>2189.919108119857</v>
       </c>
       <c r="F27">
-        <v>268154423995.2066</v>
+        <v>268154423995.2065</v>
       </c>
       <c r="G27">
-        <v>47540.34007387587</v>
+        <v>47540.34007387586</v>
       </c>
       <c r="H27">
         <v>779629570395.5896</v>
       </c>
       <c r="I27">
-        <v>6.299997474136078</v>
+        <v>6.299997474136077</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1230,7 +1230,7 @@
         <v>268300211704.0576</v>
       </c>
       <c r="G28">
-        <v>47809.47094669526</v>
+        <v>47809.47094669527</v>
       </c>
       <c r="H28">
         <v>796627744239.3857</v>
@@ -1244,13 +1244,13 @@
         <v>2017</v>
       </c>
       <c r="B29">
-        <v>66.74027625472367</v>
+        <v>66.74027625472365</v>
       </c>
       <c r="C29">
         <v>2.890655339587727</v>
       </c>
       <c r="D29">
-        <v>3.415766773460959</v>
+        <v>3.415766773460958</v>
       </c>
       <c r="E29">
         <v>2133.509215134108</v>
@@ -1259,13 +1259,13 @@
         <v>273227780611.5049</v>
       </c>
       <c r="G29">
-        <v>48510.01010601428</v>
+        <v>48510.01010601427</v>
       </c>
       <c r="H29">
-        <v>819924914198.7045</v>
+        <v>819924914198.7043</v>
       </c>
       <c r="I29">
-        <v>5.798737462442747</v>
+        <v>5.798737462442746</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1273,13 +1273,13 @@
         <v>2018</v>
       </c>
       <c r="B30">
-        <v>66.55950781501755</v>
+        <v>66.55950781501757</v>
       </c>
       <c r="C30">
         <v>2.931334804073324</v>
       </c>
       <c r="D30">
-        <v>3.51564834267282</v>
+        <v>3.515648342672821</v>
       </c>
       <c r="E30">
         <v>2121.452572318703</v>
@@ -1288,13 +1288,13 @@
         <v>281383629855.2997</v>
       </c>
       <c r="G30">
-        <v>49497.43137320487</v>
+        <v>49497.43137320488</v>
       </c>
       <c r="H30">
-        <v>848704211863.9331</v>
+        <v>848704211863.9333</v>
       </c>
       <c r="I30">
-        <v>5.777271824567839</v>
+        <v>5.77727182456784</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1302,13 +1302,13 @@
         <v>2019</v>
       </c>
       <c r="B31">
-        <v>66.36029076749838</v>
+        <v>66.3602907674984</v>
       </c>
       <c r="C31">
         <v>2.972891614093306</v>
       </c>
       <c r="D31">
-        <v>3.435496897242811</v>
+        <v>3.435496897242812</v>
       </c>
       <c r="E31">
         <v>2099.865418928516</v>
@@ -1320,10 +1320,10 @@
         <v>50107.4911549368</v>
       </c>
       <c r="H31">
-        <v>869620112484.7119</v>
+        <v>869620112484.712</v>
       </c>
       <c r="I31">
-        <v>5.615118064276127</v>
+        <v>5.615118064276128</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1352,7 +1352,7 @@
         <v>882096485441.7531</v>
       </c>
       <c r="I32">
-        <v>5.651114209643661</v>
+        <v>5.65111420964366</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1431,19 +1431,19 @@
         <v>1980</v>
       </c>
       <c r="B2">
-        <v>57.9794437021311</v>
+        <v>57.97944370213111</v>
       </c>
       <c r="C2">
         <v>14.44029556815272</v>
       </c>
       <c r="D2">
-        <v>0.8049925888297378</v>
+        <v>0.804992588829738</v>
       </c>
       <c r="E2">
         <v>588.200012207</v>
       </c>
       <c r="F2">
-        <v>93051936803.53665</v>
+        <v>93051936803.53667</v>
       </c>
       <c r="G2">
         <v>1966.903626442022</v>
@@ -1452,7 +1452,7 @@
         <v>185449993606.2382</v>
       </c>
       <c r="I2">
-        <v>29.94925716914291</v>
+        <v>29.94925716914292</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1460,13 +1460,13 @@
         <v>1981</v>
       </c>
       <c r="B3">
-        <v>58.10012592737771</v>
+        <v>58.10012592737773</v>
       </c>
       <c r="C3">
         <v>14.62237672357245</v>
       </c>
       <c r="D3">
-        <v>0.8958360552710949</v>
+        <v>0.895836055271095</v>
       </c>
       <c r="E3">
         <v>618.2000186657831</v>
@@ -1475,7 +1475,7 @@
         <v>98542118430.82996</v>
       </c>
       <c r="G3">
-        <v>2030.977203196403</v>
+        <v>2030.977203196404</v>
       </c>
       <c r="H3">
         <v>195116392922.2778</v>
@@ -1489,13 +1489,13 @@
         <v>1982</v>
       </c>
       <c r="B4">
-        <v>58.2348938918423</v>
+        <v>58.23489389184231</v>
       </c>
       <c r="C4">
         <v>14.81340942404421</v>
       </c>
       <c r="D4">
-        <v>0.961725280323424</v>
+        <v>0.9617252803234241</v>
       </c>
       <c r="E4">
         <v>661.6361297508347</v>
@@ -1530,7 +1530,7 @@
         <v>670.6302913209313</v>
       </c>
       <c r="F5">
-        <v>97591948801.97604</v>
+        <v>97591948801.97601</v>
       </c>
       <c r="G5">
         <v>1893.819319839666</v>
@@ -1547,28 +1547,28 @@
         <v>1984</v>
       </c>
       <c r="B6">
-        <v>58.53145811276157</v>
+        <v>58.53145811276156</v>
       </c>
       <c r="C6">
         <v>15.21835143476535</v>
       </c>
       <c r="D6">
-        <v>0.9078543384712789</v>
+        <v>0.9078543384712788</v>
       </c>
       <c r="E6">
-        <v>710.7523651868382</v>
+        <v>710.7523651868381</v>
       </c>
       <c r="F6">
-        <v>94981530217.25873</v>
+        <v>94981530217.25871</v>
       </c>
       <c r="G6">
         <v>1776.460641546395</v>
       </c>
       <c r="H6">
-        <v>186391898463.4151</v>
+        <v>186391898463.415</v>
       </c>
       <c r="I6">
-        <v>34.27124671763331</v>
+        <v>34.2712467176333</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1585,7 +1585,7 @@
         <v>0.8882432542679786</v>
       </c>
       <c r="E7">
-        <v>754.1488448404912</v>
+        <v>754.1488448404913</v>
       </c>
       <c r="F7">
         <v>91003248638.21613</v>
@@ -1605,7 +1605,7 @@
         <v>1986</v>
       </c>
       <c r="B8">
-        <v>58.83973635502757</v>
+        <v>58.83973635502756</v>
       </c>
       <c r="C8">
         <v>15.64549979791241</v>
@@ -1634,7 +1634,7 @@
         <v>1987</v>
       </c>
       <c r="B9">
-        <v>58.99384176458838</v>
+        <v>58.99384176458837</v>
       </c>
       <c r="C9">
         <v>15.8652514976396</v>
@@ -1643,7 +1643,7 @@
         <v>0.6987771040259528</v>
       </c>
       <c r="E9">
-        <v>843.2558131117207</v>
+        <v>843.2558131117206</v>
       </c>
       <c r="F9">
         <v>92932842624.54953</v>
@@ -1669,13 +1669,13 @@
         <v>16.08857161897359</v>
       </c>
       <c r="D10">
-        <v>0.7639019322172117</v>
+        <v>0.7639019322172119</v>
       </c>
       <c r="E10">
         <v>865.6986714699763</v>
       </c>
       <c r="F10">
-        <v>95721270368.52663</v>
+        <v>95721270368.52664</v>
       </c>
       <c r="G10">
         <v>1681.871285158689</v>
@@ -1684,7 +1684,7 @@
         <v>181582017977.1679</v>
       </c>
       <c r="I10">
-        <v>29.978592167725</v>
+        <v>29.97859216772501</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1692,16 +1692,16 @@
         <v>1989</v>
       </c>
       <c r="B11">
-        <v>59.33557879251425</v>
+        <v>59.33557879251426</v>
       </c>
       <c r="C11">
         <v>16.31533988988851</v>
       </c>
       <c r="D11">
-        <v>0.6938927808915448</v>
+        <v>0.693892780891545</v>
       </c>
       <c r="E11">
-        <v>910.8060888484157</v>
+        <v>910.8060888484158</v>
       </c>
       <c r="F11">
         <v>103875654960.067</v>
@@ -1710,7 +1710,7 @@
         <v>1792.113941744396</v>
       </c>
       <c r="H11">
-        <v>191180446552.1798</v>
+        <v>191180446552.1799</v>
       </c>
       <c r="I11">
         <v>29.26089572859051</v>
@@ -1721,7 +1721,7 @@
         <v>1990</v>
       </c>
       <c r="B12">
-        <v>59.52498065260457</v>
+        <v>59.52498065260456</v>
       </c>
       <c r="C12">
         <v>16.5455428608068</v>
@@ -1730,7 +1730,7 @@
         <v>0.6267837153889414</v>
       </c>
       <c r="E12">
-        <v>936.8708381066971</v>
+        <v>936.8708381066969</v>
       </c>
       <c r="F12">
         <v>107853429372.6698</v>
@@ -1742,7 +1742,7 @@
         <v>208827180064.5034</v>
       </c>
       <c r="I12">
-        <v>22.82812987817549</v>
+        <v>22.82812987817548</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1759,7 +1759,7 @@
         <v>0.582252164774663</v>
       </c>
       <c r="E13">
-        <v>946.8670008397249</v>
+        <v>946.8670008397252</v>
       </c>
       <c r="F13">
         <v>107997183813.9955</v>
@@ -1779,7 +1779,7 @@
         <v>1992</v>
       </c>
       <c r="B14">
-        <v>59.94978248318462</v>
+        <v>59.94978248318461</v>
       </c>
       <c r="C14">
         <v>17.01548044262723</v>
@@ -1826,7 +1826,7 @@
         <v>2039.601401614884</v>
       </c>
       <c r="H15">
-        <v>232271208240.1212</v>
+        <v>232271208240.1211</v>
       </c>
       <c r="I15">
         <v>26.04973651086909</v>
@@ -1843,7 +1843,7 @@
         <v>17.49732010969391</v>
       </c>
       <c r="D16">
-        <v>0.5599722807195595</v>
+        <v>0.5599722807195594</v>
       </c>
       <c r="E16">
         <v>1077.06728228633</v>
@@ -1855,7 +1855,7 @@
         <v>2206.842264760318</v>
       </c>
       <c r="H16">
-        <v>255567231304.0632</v>
+        <v>255567231304.0633</v>
       </c>
       <c r="I16">
         <v>23.72123370088062</v>
@@ -1866,7 +1866,7 @@
         <v>1995</v>
       </c>
       <c r="B17">
-        <v>60.69481798557469</v>
+        <v>60.6948179855747</v>
       </c>
       <c r="C17">
         <v>17.74300273329708</v>
@@ -1901,7 +1901,7 @@
         <v>17.99209167666523</v>
       </c>
       <c r="D18">
-        <v>0.6849842526307558</v>
+        <v>0.6849842526307559</v>
       </c>
       <c r="E18">
         <v>1206.839284682198</v>
@@ -1913,7 +1913,7 @@
         <v>2873.07200840935</v>
       </c>
       <c r="H18">
-        <v>360013884915.0398</v>
+        <v>360013884915.0399</v>
       </c>
       <c r="I18">
         <v>13.06719123672183</v>
@@ -1930,7 +1930,7 @@
         <v>18.24456070193941</v>
       </c>
       <c r="D19">
-        <v>0.8687419315670456</v>
+        <v>0.8687419315670455</v>
       </c>
       <c r="E19">
         <v>1279.950316690565</v>
@@ -1968,7 +1968,7 @@
         <v>150916260179.9922</v>
       </c>
       <c r="G20">
-        <v>3411.245612786299</v>
+        <v>3411.245612786298</v>
       </c>
       <c r="H20">
         <v>448168704007.1182</v>
@@ -2000,7 +2000,7 @@
         <v>3419.604113757096</v>
       </c>
       <c r="H21">
-        <v>455273107752.8575</v>
+        <v>455273107752.8574</v>
       </c>
       <c r="I21">
         <v>12.3085333305115</v>
@@ -2011,7 +2011,7 @@
         <v>2000</v>
       </c>
       <c r="B22">
-        <v>62.28189411285897</v>
+        <v>62.28189411285898</v>
       </c>
       <c r="C22">
         <v>19.0174673092937</v>
@@ -2026,10 +2026,10 @@
         <v>148703279214.5289</v>
       </c>
       <c r="G22">
-        <v>3459.379833210767</v>
+        <v>3459.379833210768</v>
       </c>
       <c r="H22">
-        <v>466244874936.8907</v>
+        <v>466244874936.8906</v>
       </c>
       <c r="I22">
         <v>13.13465959355212</v>
@@ -2069,7 +2069,7 @@
         <v>2002</v>
       </c>
       <c r="B24">
-        <v>62.97036460689064</v>
+        <v>62.97036460689063</v>
       </c>
       <c r="C24">
         <v>19.5377827495895</v>
@@ -2127,7 +2127,7 @@
         <v>2004</v>
       </c>
       <c r="B26">
-        <v>63.65880999885195</v>
+        <v>63.65880999885196</v>
       </c>
       <c r="C26">
         <v>20.05520282606226</v>
@@ -2156,7 +2156,7 @@
         <v>2005</v>
       </c>
       <c r="B27">
-        <v>64.00255917134332</v>
+        <v>64.00255917134334</v>
       </c>
       <c r="C27">
         <v>20.3110808150638</v>
@@ -2185,7 +2185,7 @@
         <v>2006</v>
       </c>
       <c r="B28">
-        <v>64.34772847109147</v>
+        <v>64.34772847109146</v>
       </c>
       <c r="C28">
         <v>20.56418411558038</v>
@@ -2200,7 +2200,7 @@
         <v>164226068226.4986</v>
       </c>
       <c r="G28">
-        <v>3795.295820295331</v>
+        <v>3795.29582029533</v>
       </c>
       <c r="H28">
         <v>539359656681.5369</v>
@@ -2229,10 +2229,10 @@
         <v>182396354714.699</v>
       </c>
       <c r="G29">
-        <v>4201.668030940149</v>
+        <v>4201.668030940148</v>
       </c>
       <c r="H29">
-        <v>603619078232.5284</v>
+        <v>603619078232.5283</v>
       </c>
       <c r="I29">
         <v>14.1542648058524</v>
@@ -2249,7 +2249,7 @@
         <v>21.06008377390752</v>
       </c>
       <c r="D30">
-        <v>2.415686069851729</v>
+        <v>2.415686069851728</v>
       </c>
       <c r="E30">
         <v>1484.812295733213</v>
@@ -2319,7 +2319,7 @@
         <v>5859.439141998546</v>
       </c>
       <c r="H32">
-        <v>874654964786.4541</v>
+        <v>874654964786.454</v>
       </c>
       <c r="I32">
         <v>12.72185960924913</v>
@@ -2330,7 +2330,7 @@
         <v>2011</v>
       </c>
       <c r="B33">
-        <v>66.04304687473932</v>
+        <v>66.0430468747393</v>
       </c>
       <c r="C33">
         <v>21.77700281498143</v>
@@ -2400,7 +2400,7 @@
         <v>1479.420128756364</v>
       </c>
       <c r="F35">
-        <v>346659144424.9864</v>
+        <v>346659144424.9863</v>
       </c>
       <c r="G35">
         <v>7887.471791051108</v>
@@ -2417,7 +2417,7 @@
         <v>2014</v>
       </c>
       <c r="B36">
-        <v>66.98522354847182</v>
+        <v>66.98522354847181</v>
       </c>
       <c r="C36">
         <v>22.46455768861505</v>
@@ -2429,10 +2429,10 @@
         <v>1492.551362945261</v>
       </c>
       <c r="F36">
-        <v>364131837623.6959</v>
+        <v>364131837623.696</v>
       </c>
       <c r="G36">
-        <v>8360.266021504443</v>
+        <v>8360.266021504445</v>
       </c>
       <c r="H36">
         <v>1304914147709.545</v>
@@ -2519,7 +2519,7 @@
         <v>360613288820.9044</v>
       </c>
       <c r="G39">
-        <v>8609.544794734609</v>
+        <v>8609.544794734607</v>
       </c>
       <c r="H39">
         <v>1393416319211.512</v>
@@ -2533,22 +2533,22 @@
         <v>2018</v>
       </c>
       <c r="B40">
-        <v>67.99839217160422</v>
+        <v>67.99839217160424</v>
       </c>
       <c r="C40">
-        <v>23.34152464111731</v>
+        <v>23.34152464111732</v>
       </c>
       <c r="D40">
-        <v>3.239770314598544</v>
+        <v>3.239770314598545</v>
       </c>
       <c r="E40">
         <v>1557.935762747051</v>
       </c>
       <c r="F40">
-        <v>360479159927.5264</v>
+        <v>360479159927.5265</v>
       </c>
       <c r="G40">
-        <v>8669.786753717553</v>
+        <v>8669.786753717555</v>
       </c>
       <c r="H40">
         <v>1418610667181.579</v>
@@ -2577,7 +2577,7 @@
         <v>359462949359.974</v>
       </c>
       <c r="G41">
-        <v>8692.693344014668</v>
+        <v>8692.693344014669</v>
       </c>
       <c r="H41">
         <v>1438163779052.4</v>
@@ -2651,7 +2651,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2703,34 +2703,34 @@
         <v>1997</v>
       </c>
       <c r="B2">
-        <v>32.6699981689453</v>
+        <v>32.66999816894531</v>
       </c>
       <c r="C2">
         <v>1.61386001110077</v>
       </c>
       <c r="D2">
-        <v>3132.90307617188</v>
+        <v>3132.903076171881</v>
       </c>
       <c r="E2">
-        <v>67.75619383813979</v>
+        <v>67.75619383813981</v>
       </c>
       <c r="F2">
-        <v>3.335636360797226</v>
+        <v>3.335636360797227</v>
       </c>
       <c r="G2">
-        <v>2.317969734519726</v>
+        <v>2.317969734519727</v>
       </c>
       <c r="H2">
         <v>1956.5</v>
       </c>
       <c r="I2">
-        <v>181539072656.3629</v>
+        <v>181539072656.363</v>
       </c>
       <c r="J2">
-        <v>21901.56285483924</v>
+        <v>21901.56285483925</v>
       </c>
       <c r="K2">
-        <v>502570417449.0828</v>
+        <v>502570417449.0829</v>
       </c>
       <c r="L2">
         <v>23.0599994659424</v>
@@ -2744,7 +2744,7 @@
         <v>1998</v>
       </c>
       <c r="B3">
-        <v>32.78518205413017</v>
+        <v>32.78518205413016</v>
       </c>
       <c r="C3">
         <v>1.664462107638414</v>
@@ -2785,7 +2785,7 @@
         <v>1999</v>
       </c>
       <c r="B4">
-        <v>32.82346310139587</v>
+        <v>32.82346310139588</v>
       </c>
       <c r="C4">
         <v>1.695647209378795</v>
@@ -2812,7 +2812,7 @@
         <v>21761.18596317444</v>
       </c>
       <c r="K4">
-        <v>501306453302.753</v>
+        <v>501306453302.7531</v>
       </c>
       <c r="L4">
         <v>23.10185426415496</v>
@@ -2841,7 +2841,7 @@
         <v>3.3815372655734</v>
       </c>
       <c r="G5">
-        <v>5.115976335518152</v>
+        <v>5.115976335518153</v>
       </c>
       <c r="H5">
         <v>1883.920841582331</v>
@@ -2873,7 +2873,7 @@
         <v>1.809042664124698</v>
       </c>
       <c r="D6">
-        <v>3387.824453801564</v>
+        <v>3387.824453801563</v>
       </c>
       <c r="E6">
         <v>68.1387512429104</v>
@@ -2882,7 +2882,7 @@
         <v>3.400318793020999</v>
       </c>
       <c r="G6">
-        <v>4.810990277963039</v>
+        <v>4.810990277963038</v>
       </c>
       <c r="H6">
         <v>1842.242529093149</v>
@@ -2894,7 +2894,7 @@
         <v>22801.25523202907</v>
       </c>
       <c r="K6">
-        <v>523547032590.3589</v>
+        <v>523547032590.3588</v>
       </c>
       <c r="L6">
         <v>23.13282041925713</v>
@@ -2923,7 +2923,7 @@
         <v>3.420626768779385</v>
       </c>
       <c r="G7">
-        <v>4.479456744034007</v>
+        <v>4.479456744034006</v>
       </c>
       <c r="H7">
         <v>1787.21428190015</v>
@@ -2958,7 +2958,7 @@
         <v>3541.9087574357</v>
       </c>
       <c r="E8">
-        <v>68.36711586469087</v>
+        <v>68.36711586469086</v>
       </c>
       <c r="F8">
         <v>3.440903218551935</v>
@@ -2999,7 +2999,7 @@
         <v>3636.384941007966</v>
       </c>
       <c r="E9">
-        <v>68.48218497343315</v>
+        <v>68.48218497343314</v>
       </c>
       <c r="F9">
         <v>3.461575606012826</v>
@@ -3014,7 +3014,7 @@
         <v>222575716580.8365</v>
       </c>
       <c r="J9">
-        <v>25443.22132125172</v>
+        <v>25443.22132125171</v>
       </c>
       <c r="K9">
         <v>595052268464.1143</v>
@@ -3043,7 +3043,7 @@
         <v>68.59613688012247</v>
       </c>
       <c r="F10">
-        <v>3.482784966437911</v>
+        <v>3.482784966437912</v>
       </c>
       <c r="G10">
         <v>3.014787796913335</v>
@@ -3055,10 +3055,10 @@
         <v>241474089381.8195</v>
       </c>
       <c r="J10">
-        <v>27164.22652968862</v>
+        <v>27164.22652968863</v>
       </c>
       <c r="K10">
-        <v>636868453987.4408</v>
+        <v>636868453987.4409</v>
       </c>
       <c r="L10">
         <v>23.04160623696955</v>
@@ -3081,13 +3081,13 @@
         <v>3819.917323621261</v>
       </c>
       <c r="E11">
-        <v>68.70435847289001</v>
+        <v>68.70435847289002</v>
       </c>
       <c r="F11">
         <v>3.504913256198078</v>
       </c>
       <c r="G11">
-        <v>3.288850410262443</v>
+        <v>3.288850410262444</v>
       </c>
       <c r="H11">
         <v>1662.160963948937</v>
@@ -3113,7 +3113,7 @@
         <v>2007</v>
       </c>
       <c r="B12">
-        <v>32.83163251908109</v>
+        <v>32.8316325190811</v>
       </c>
       <c r="C12">
         <v>1.907053006150764</v>
@@ -3122,10 +3122,10 @@
         <v>3928.017704004435</v>
       </c>
       <c r="E12">
-        <v>68.80518824631935</v>
+        <v>68.80518824631933</v>
       </c>
       <c r="F12">
-        <v>3.527697683450297</v>
+        <v>3.527697683450296</v>
       </c>
       <c r="G12">
         <v>3.973534927901461</v>
@@ -3140,7 +3140,7 @@
         <v>31295.28780461649</v>
       </c>
       <c r="K12">
-        <v>742058489360.2648</v>
+        <v>742058489360.2646</v>
       </c>
       <c r="L12">
         <v>22.73222990217566</v>
@@ -3169,13 +3169,13 @@
         <v>3.551688572352852</v>
       </c>
       <c r="G13">
-        <v>4.045479482432167</v>
+        <v>4.045479482432168</v>
       </c>
       <c r="H13">
         <v>1597.74807055232</v>
       </c>
       <c r="I13">
-        <v>306972644090.5034</v>
+        <v>306972644090.5035</v>
       </c>
       <c r="J13">
         <v>33342.99172328279</v>
@@ -3201,7 +3201,7 @@
         <v>1.902430206498004</v>
       </c>
       <c r="D14">
-        <v>4085.965168026008</v>
+        <v>4085.965168026009</v>
       </c>
       <c r="E14">
         <v>68.96584160530999</v>
@@ -3222,7 +3222,7 @@
         <v>34302.58586874815</v>
       </c>
       <c r="K14">
-        <v>834326051358.703</v>
+        <v>834326051358.7029</v>
       </c>
       <c r="L14">
         <v>22.27366709992755</v>
@@ -3239,13 +3239,13 @@
         <v>32.22781171149491</v>
       </c>
       <c r="C15">
-        <v>1.892956918092349</v>
+        <v>1.892956918092348</v>
       </c>
       <c r="D15">
-        <v>4154.769379638839</v>
+        <v>4154.769379638838</v>
       </c>
       <c r="E15">
-        <v>69.01396693194717</v>
+        <v>69.01396693194715</v>
       </c>
       <c r="F15">
         <v>3.603555384372446</v>
@@ -3289,7 +3289,7 @@
         <v>69.02818065635608</v>
       </c>
       <c r="F16">
-        <v>3.630492585895168</v>
+        <v>3.630492585895169</v>
       </c>
       <c r="G16">
         <v>3.331528293901755</v>
@@ -3304,13 +3304,13 @@
         <v>37867.81958006493</v>
       </c>
       <c r="K16">
-        <v>946456868743.7018</v>
+        <v>946456868743.7019</v>
       </c>
       <c r="L16">
         <v>21.80806322954592</v>
       </c>
       <c r="M16">
-        <v>9.95539617251473</v>
+        <v>9.955396172514728</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -3318,7 +3318,7 @@
         <v>2012</v>
       </c>
       <c r="B17">
-        <v>31.87924323548698</v>
+        <v>31.87924323548699</v>
       </c>
       <c r="C17">
         <v>1.867889948180352</v>
@@ -3330,22 +3330,22 @@
         <v>69.01329728770965</v>
       </c>
       <c r="F17">
-        <v>3.658392529681702</v>
+        <v>3.658392529681703</v>
       </c>
       <c r="G17">
-        <v>3.258572757786065</v>
+        <v>3.258572757786066</v>
       </c>
       <c r="H17">
         <v>1692.370659126793</v>
       </c>
       <c r="I17">
-        <v>361364604086.8269</v>
+        <v>361364604086.827</v>
       </c>
       <c r="J17">
         <v>39578.15257388676</v>
       </c>
       <c r="K17">
-        <v>999936514975.0247</v>
+        <v>999936514975.0248</v>
       </c>
       <c r="L17">
         <v>21.65229020970236</v>
@@ -3371,16 +3371,16 @@
         <v>68.97021048890358</v>
       </c>
       <c r="F18">
-        <v>3.687087703709614</v>
+        <v>3.687087703709615</v>
       </c>
       <c r="G18">
         <v>3.300400846466616</v>
       </c>
       <c r="H18">
-        <v>1720.982511710717</v>
+        <v>1720.982511710718</v>
       </c>
       <c r="I18">
-        <v>376020635556.0294</v>
+        <v>376020635556.0295</v>
       </c>
       <c r="J18">
         <v>41049.33886495115</v>
@@ -3392,7 +3392,7 @@
         <v>21.50330253974739</v>
       </c>
       <c r="M18">
-        <v>9.588492358255939</v>
+        <v>9.588492358255941</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -3421,7 +3421,7 @@
         <v>1761.013318304308</v>
       </c>
       <c r="I19">
-        <v>388583184077.8258</v>
+        <v>388583184077.8257</v>
       </c>
       <c r="J19">
         <v>42140.81328359441</v>
@@ -3447,31 +3447,31 @@
         <v>1.819389294626783</v>
       </c>
       <c r="D20">
-        <v>4359.275951967618</v>
+        <v>4359.275951967619</v>
       </c>
       <c r="E20">
-        <v>68.7961750355627</v>
+        <v>68.79617503556271</v>
       </c>
       <c r="F20">
-        <v>3.745054831554355</v>
+        <v>3.745054831554357</v>
       </c>
       <c r="G20">
         <v>3.385089963675099</v>
       </c>
       <c r="H20">
-        <v>1794.90464287317</v>
+        <v>1794.904642873171</v>
       </c>
       <c r="I20">
         <v>387659709837.535</v>
       </c>
       <c r="J20">
-        <v>42297.98357831326</v>
+        <v>42297.98357831327</v>
       </c>
       <c r="K20">
         <v>1098113225590.742</v>
       </c>
       <c r="L20">
-        <v>21.20226036580292</v>
+        <v>21.20226036580293</v>
       </c>
       <c r="M20">
         <v>9.975422544339398</v>
@@ -3488,22 +3488,22 @@
         <v>1.809771458953148</v>
       </c>
       <c r="D21">
-        <v>4360.374376189237</v>
+        <v>4360.374376189238</v>
       </c>
       <c r="E21">
-        <v>68.67425705065963</v>
+        <v>68.67425705065965</v>
       </c>
       <c r="F21">
-        <v>3.775025559971698</v>
+        <v>3.775025559971699</v>
       </c>
       <c r="G21">
         <v>3.263435025322558</v>
       </c>
       <c r="H21">
-        <v>1842.784382581193</v>
+        <v>1842.784382581194</v>
       </c>
       <c r="I21">
-        <v>384295803781.0363</v>
+        <v>384295803781.0364</v>
       </c>
       <c r="J21">
         <v>42299.85285626946</v>
@@ -3515,7 +3515,7 @@
         <v>21.03970646805755</v>
       </c>
       <c r="M21">
-        <v>9.928004135207868</v>
+        <v>9.928004135207869</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -3544,7 +3544,7 @@
         <v>1947.004500449027</v>
       </c>
       <c r="I22">
-        <v>385547289362.4151</v>
+        <v>385547289362.4152</v>
       </c>
       <c r="J22">
         <v>42595.28319887476</v>
@@ -3556,7 +3556,7 @@
         <v>20.88208114659832</v>
       </c>
       <c r="M22">
-        <v>9.68457578828024</v>
+        <v>9.684575788280242</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -3598,6 +3598,129 @@
       </c>
       <c r="M23">
         <v>9.866071588318858</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24">
+        <v>2019</v>
+      </c>
+      <c r="B24">
+        <v>30.88947112150036</v>
+      </c>
+      <c r="C24">
+        <v>1.782475471741764</v>
+      </c>
+      <c r="D24">
+        <v>4401.189022169747</v>
+      </c>
+      <c r="E24">
+        <v>68.17190772618737</v>
+      </c>
+      <c r="F24">
+        <v>3.877355069028355</v>
+      </c>
+      <c r="G24">
+        <v>3.234966632405808</v>
+      </c>
+      <c r="H24">
+        <v>1862.20950601299</v>
+      </c>
+      <c r="I24">
+        <v>392987038651.9529</v>
+      </c>
+      <c r="J24">
+        <v>43220.57599156904</v>
+      </c>
+      <c r="K24">
+        <v>1173777444673.934</v>
+      </c>
+      <c r="L24">
+        <v>20.653344976093</v>
+      </c>
+      <c r="M24">
+        <v>11.00002937864495</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25">
+        <v>2020</v>
+      </c>
+      <c r="B25">
+        <v>30.9373758269501</v>
+      </c>
+      <c r="C25">
+        <v>1.79913435464459</v>
+      </c>
+      <c r="D25">
+        <v>4418.36223891603</v>
+      </c>
+      <c r="E25">
+        <v>67.96211361342688</v>
+      </c>
+      <c r="F25">
+        <v>3.919100619222935</v>
+      </c>
+      <c r="G25">
+        <v>3.889088608162179</v>
+      </c>
+      <c r="H25">
+        <v>1381.658065493557</v>
+      </c>
+      <c r="I25">
+        <v>392307475576.6382</v>
+      </c>
+      <c r="J25">
+        <v>42950.48943015601</v>
+      </c>
+      <c r="K25">
+        <v>1185817904568.241</v>
+      </c>
+      <c r="L25">
+        <v>20.61978729953481</v>
+      </c>
+      <c r="M25">
+        <v>13.61398700257975</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>2021</v>
+      </c>
+      <c r="B26">
+        <v>31.15330046471943</v>
+      </c>
+      <c r="C26">
+        <v>1.843728379660454</v>
+      </c>
+      <c r="D26">
+        <v>4428.440076965558</v>
+      </c>
+      <c r="E26">
+        <v>67.73362424761586</v>
+      </c>
+      <c r="F26">
+        <v>3.966579888247957</v>
+      </c>
+      <c r="G26">
+        <v>5.143509585549259</v>
+      </c>
+      <c r="H26">
+        <v>414.6464439628072</v>
+      </c>
+      <c r="I26">
+        <v>384116402832.2852</v>
+      </c>
+      <c r="J26">
+        <v>41891.94822256824</v>
+      </c>
+      <c r="K26">
+        <v>1183231889096.639</v>
+      </c>
+      <c r="L26">
+        <v>20.66513867709819</v>
+      </c>
+      <c r="M26">
+        <v>18.23548230344448</v>
       </c>
     </row>
   </sheetData>
@@ -3671,13 +3794,13 @@
         <v>700.070129394531</v>
       </c>
       <c r="E2">
-        <v>71.5088523199023</v>
+        <v>71.50885231990232</v>
       </c>
       <c r="F2">
         <v>137.5189588252698</v>
       </c>
       <c r="G2">
-        <v>3.483641113737494</v>
+        <v>3.483641113737495</v>
       </c>
       <c r="H2">
         <v>7024.25</v>
@@ -3686,7 +3809,7 @@
         <v>74725444</v>
       </c>
       <c r="J2">
-        <v>897508414097.2357</v>
+        <v>897508414097.2358</v>
       </c>
       <c r="K2">
         <v>1508.668097884526</v>
@@ -3712,7 +3835,7 @@
         <v>1.263386242091658</v>
       </c>
       <c r="D3">
-        <v>773.2813224792483</v>
+        <v>773.2813224792484</v>
       </c>
       <c r="E3">
         <v>71.85011660025272</v>
@@ -3724,13 +3847,13 @@
         <v>4.041252009667088</v>
       </c>
       <c r="H3">
-        <v>7313.391145833333</v>
+        <v>7313.391145833334</v>
       </c>
       <c r="I3">
-        <v>70829516.39583334</v>
+        <v>70829516.39583336</v>
       </c>
       <c r="J3">
-        <v>989910336842.761</v>
+        <v>989910336842.7612</v>
       </c>
       <c r="K3">
         <v>1636.141916309794</v>
@@ -3750,13 +3873,13 @@
         <v>2006</v>
       </c>
       <c r="B4">
-        <v>24.60776736654943</v>
+        <v>24.60776736654944</v>
       </c>
       <c r="C4">
         <v>1.301397305751137</v>
       </c>
       <c r="D4">
-        <v>824.270185833518</v>
+        <v>824.2701858335181</v>
       </c>
       <c r="E4">
         <v>72.14778266964144</v>
@@ -3768,7 +3891,7 @@
         <v>4.210181667724007</v>
       </c>
       <c r="H4">
-        <v>7450.325014459226</v>
+        <v>7450.325014459227</v>
       </c>
       <c r="I4">
         <v>75883372.16657028</v>
@@ -3786,7 +3909,7 @@
         <v>23.9083285356547</v>
       </c>
       <c r="N4">
-        <v>32.45232805659434</v>
+        <v>32.45232805659435</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3800,7 +3923,7 @@
         <v>1.321789663674549</v>
       </c>
       <c r="D5">
-        <v>890.0581716133102</v>
+        <v>890.0581716133103</v>
       </c>
       <c r="E5">
         <v>72.38404878917351</v>
@@ -3812,7 +3935,7 @@
         <v>4.263997867028277</v>
       </c>
       <c r="H5">
-        <v>8505.083876733102</v>
+        <v>8505.083876733101</v>
       </c>
       <c r="I5">
         <v>83764601.58412766</v>
@@ -3830,7 +3953,7 @@
         <v>24.72401229340791</v>
       </c>
       <c r="N5">
-        <v>32.38335311644068</v>
+        <v>32.38335311644067</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3844,10 +3967,10 @@
         <v>1.350918111749324</v>
       </c>
       <c r="D6">
-        <v>957.2652172089264</v>
+        <v>957.2652172089261</v>
       </c>
       <c r="E6">
-        <v>72.559002635933</v>
+        <v>72.55900263593298</v>
       </c>
       <c r="F6">
         <v>139.1933278300434</v>
@@ -3856,10 +3979,10 @@
         <v>4.139542781505694</v>
       </c>
       <c r="H6">
-        <v>9181.133154040423</v>
+        <v>9181.133154040421</v>
       </c>
       <c r="I6">
-        <v>91315349.48559719</v>
+        <v>91315349.48559718</v>
       </c>
       <c r="J6">
         <v>1473005490748.256</v>
@@ -3888,7 +4011,7 @@
         <v>1.414707960409268</v>
       </c>
       <c r="D7">
-        <v>934.7666416346091</v>
+        <v>934.766641634609</v>
       </c>
       <c r="E7">
         <v>72.69043535439154</v>
@@ -3897,19 +4020,19 @@
         <v>139.6117568478471</v>
       </c>
       <c r="G7">
-        <v>3.820340556923639</v>
+        <v>3.820340556923638</v>
       </c>
       <c r="H7">
-        <v>9749.219598527903</v>
+        <v>9749.219598527901</v>
       </c>
       <c r="I7">
-        <v>94868720.52781025</v>
+        <v>94868720.52781023</v>
       </c>
       <c r="J7">
         <v>1650138025419.663</v>
       </c>
       <c r="K7">
-        <v>2680.256413739259</v>
+        <v>2680.256413739258</v>
       </c>
       <c r="L7">
         <v>1812867911357.006</v>
@@ -3918,7 +4041,7 @@
         <v>25.81207821146122</v>
       </c>
       <c r="N7">
-        <v>31.59623809103104</v>
+        <v>31.59623809103103</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -3935,7 +4058,7 @@
         <v>925.6886595612642</v>
       </c>
       <c r="E8">
-        <v>72.79449953325198</v>
+        <v>72.79449953325199</v>
       </c>
       <c r="F8">
         <v>140.0323014756228</v>
@@ -3976,10 +4099,10 @@
         <v>1.520007529985069</v>
       </c>
       <c r="D9">
-        <v>930.9273742313422</v>
+        <v>930.9273742313421</v>
       </c>
       <c r="E9">
-        <v>72.86623612673057</v>
+        <v>72.86623612673056</v>
       </c>
       <c r="F9">
         <v>140.4729942112967</v>
@@ -4014,13 +4137,13 @@
         <v>2012</v>
       </c>
       <c r="B10">
-        <v>28.73316409241844</v>
+        <v>28.73316409241845</v>
       </c>
       <c r="C10">
         <v>1.579439705582359</v>
       </c>
       <c r="D10">
-        <v>943.5652540100999</v>
+        <v>943.5652540101</v>
       </c>
       <c r="E10">
         <v>72.91334019310126</v>
@@ -4044,10 +4167,10 @@
         <v>3877.995374161435</v>
       </c>
       <c r="L10">
-        <v>2624228994908.267</v>
+        <v>2624228994908.268</v>
       </c>
       <c r="M10">
-        <v>27.37697263190987</v>
+        <v>27.37697263190988</v>
       </c>
       <c r="N10">
         <v>31.52857786597396</v>
@@ -4067,13 +4190,13 @@
         <v>960.912083051752</v>
       </c>
       <c r="E11">
-        <v>72.93704395405599</v>
+        <v>72.93704395405601</v>
       </c>
       <c r="F11">
         <v>141.4811298939973</v>
       </c>
       <c r="G11">
-        <v>3.587535477110026</v>
+        <v>3.587535477110027</v>
       </c>
       <c r="H11">
         <v>13058.00574379439</v>
@@ -4102,7 +4225,7 @@
         <v>2014</v>
       </c>
       <c r="B12">
-        <v>29.64961367105322</v>
+        <v>29.64961367105321</v>
       </c>
       <c r="C12">
         <v>1.689764610740267</v>
@@ -4173,7 +4296,7 @@
         <v>3108797772578.646</v>
       </c>
       <c r="K13">
-        <v>5175.486014942855</v>
+        <v>5175.486014942854</v>
       </c>
       <c r="L13">
         <v>3631800198010.401</v>
@@ -4190,7 +4313,7 @@
         <v>2016</v>
       </c>
       <c r="B14">
-        <v>30.1293064697297</v>
+        <v>30.12930646972969</v>
       </c>
       <c r="C14">
         <v>1.780244058501921</v>
@@ -4199,13 +4322,13 @@
         <v>1023.66361719276</v>
       </c>
       <c r="E14">
-        <v>72.80851370791174</v>
+        <v>72.80851370791173</v>
       </c>
       <c r="F14">
         <v>143.14401378245</v>
       </c>
       <c r="G14">
-        <v>3.081484165643842</v>
+        <v>3.081484165643841</v>
       </c>
       <c r="H14">
         <v>15292.95442477581</v>
@@ -4217,10 +4340,10 @@
         <v>3270479267244.057</v>
       </c>
       <c r="K14">
-        <v>5528.355336888418</v>
+        <v>5528.355336888417</v>
       </c>
       <c r="L14">
-        <v>3940178316471.668</v>
+        <v>3940178316471.667</v>
       </c>
       <c r="M14">
         <v>28.26404179739093</v>
@@ -4278,7 +4401,7 @@
         <v>2018</v>
       </c>
       <c r="B16">
-        <v>30.39820630281146</v>
+        <v>30.39820630281147</v>
       </c>
       <c r="C16">
         <v>1.855262300549092</v>
@@ -4302,13 +4425,13 @@
         <v>164766352.6500916</v>
       </c>
       <c r="J16">
-        <v>3690660149830.366</v>
+        <v>3690660149830.367</v>
       </c>
       <c r="K16">
         <v>6358.115828324629</v>
       </c>
       <c r="L16">
-        <v>4646253492984.621</v>
+        <v>4646253492984.622</v>
       </c>
       <c r="M16">
         <v>28.25442883029433</v>
@@ -4322,7 +4445,7 @@
         <v>2019</v>
       </c>
       <c r="B17">
-        <v>30.44510175501271</v>
+        <v>30.44510175501272</v>
       </c>
       <c r="C17">
         <v>1.897550046515129</v>
@@ -4331,7 +4454,7 @@
         <v>1119.084802463848</v>
       </c>
       <c r="E17">
-        <v>72.32124978655806</v>
+        <v>72.32124978655804</v>
       </c>
       <c r="F17">
         <v>144.8485657501058</v>
@@ -4349,7 +4472,7 @@
         <v>3888279639578.157</v>
       </c>
       <c r="K17">
-        <v>6769.268642375135</v>
+        <v>6769.268642375136</v>
       </c>
       <c r="L17">
         <v>5010427768923.229</v>
@@ -4496,16 +4619,16 @@
         <v>1990</v>
       </c>
       <c r="B2">
-        <v>65.2851572356831</v>
+        <v>65.28515723568312</v>
       </c>
       <c r="C2">
         <v>236.6287190509651</v>
       </c>
       <c r="D2">
-        <v>3.783805679824685</v>
+        <v>3.783805679824686</v>
       </c>
       <c r="E2">
-        <v>3825.3999023438</v>
+        <v>3825.399902343801</v>
       </c>
       <c r="F2">
         <v>302806317471.5909</v>
@@ -4514,7 +4637,7 @@
         <v>19095.46699846078</v>
       </c>
       <c r="H2">
-        <v>935975374644.8864</v>
+        <v>935975374644.8866</v>
       </c>
       <c r="I2">
         <v>16.66798755183352</v>
@@ -4525,7 +4648,7 @@
         <v>1991</v>
       </c>
       <c r="B3">
-        <v>65.20839037381973</v>
+        <v>65.20839037381974</v>
       </c>
       <c r="C3">
         <v>236.9988716161741</v>
@@ -4543,7 +4666,7 @@
         <v>19502.16379242345</v>
       </c>
       <c r="H3">
-        <v>966518665201.5548</v>
+        <v>966518665201.5549</v>
       </c>
       <c r="I3">
         <v>16.26393514474525</v>
@@ -4554,13 +4677,13 @@
         <v>1992</v>
       </c>
       <c r="B4">
-        <v>65.12827694383645</v>
+        <v>65.12827694383647</v>
       </c>
       <c r="C4">
-        <v>237.3408380436418</v>
+        <v>237.3408380436419</v>
       </c>
       <c r="D4">
-        <v>2.577175206868702</v>
+        <v>2.577175206868703</v>
       </c>
       <c r="E4">
         <v>4168.15608958659</v>
@@ -4572,7 +4695,7 @@
         <v>19837.15460757254</v>
       </c>
       <c r="H4">
-        <v>993937546069.6639</v>
+        <v>993937546069.6641</v>
       </c>
       <c r="I4">
         <v>16.04603255128911</v>
@@ -4601,7 +4724,7 @@
         <v>19464.07700434617</v>
       </c>
       <c r="H5">
-        <v>981065186344.7953</v>
+        <v>981065186344.7952</v>
       </c>
       <c r="I5">
         <v>15.68185759056369</v>
@@ -4615,22 +4738,22 @@
         <v>64.97727330584169</v>
       </c>
       <c r="C6">
-        <v>237.9763845669039</v>
+        <v>237.9763845669038</v>
       </c>
       <c r="D6">
         <v>2.250368155532942</v>
       </c>
       <c r="E6">
-        <v>4886.136885233125</v>
+        <v>4886.136885233124</v>
       </c>
       <c r="F6">
-        <v>300610445068.6819</v>
+        <v>300610445068.6818</v>
       </c>
       <c r="G6">
         <v>19515.1101282385</v>
       </c>
       <c r="H6">
-        <v>986997096997.057</v>
+        <v>986997096997.0569</v>
       </c>
       <c r="I6">
         <v>16.40380812564748</v>
@@ -4653,7 +4776,7 @@
         <v>5226.799773464294</v>
       </c>
       <c r="F7">
-        <v>305893474188.9381</v>
+        <v>305893474188.9382</v>
       </c>
       <c r="G7">
         <v>20161.84022984325</v>
@@ -4679,7 +4802,7 @@
         <v>2.241967387616137</v>
       </c>
       <c r="E8">
-        <v>5589.462900461549</v>
+        <v>5589.462900461548</v>
       </c>
       <c r="F8">
         <v>312701651435.7896</v>
@@ -4699,13 +4822,13 @@
         <v>1997</v>
       </c>
       <c r="B9">
-        <v>64.85337649803331</v>
+        <v>64.8533764980333</v>
       </c>
       <c r="C9">
-        <v>238.9471942437609</v>
+        <v>238.9471942437608</v>
       </c>
       <c r="D9">
-        <v>2.382436731762102</v>
+        <v>2.382436731762101</v>
       </c>
       <c r="E9">
         <v>5704.86823928472</v>
@@ -4728,19 +4851,19 @@
         <v>1998</v>
       </c>
       <c r="B10">
-        <v>64.8465315695195</v>
+        <v>64.84653156951951</v>
       </c>
       <c r="C10">
-        <v>239.2846495440093</v>
+        <v>239.2846495440094</v>
       </c>
       <c r="D10">
         <v>2.894853594474573</v>
       </c>
       <c r="E10">
-        <v>5579.592543435145</v>
+        <v>5579.592543435146</v>
       </c>
       <c r="F10">
-        <v>327867544498.3388</v>
+        <v>327867544498.3389</v>
       </c>
       <c r="G10">
         <v>22407.14389881206</v>
@@ -4757,7 +4880,7 @@
         <v>1999</v>
       </c>
       <c r="B11">
-        <v>64.85525839077744</v>
+        <v>64.85525839077745</v>
       </c>
       <c r="C11">
         <v>239.6427200112729</v>
@@ -4766,7 +4889,7 @@
         <v>3.420784971876552</v>
       </c>
       <c r="E11">
-        <v>5508.045789014618</v>
+        <v>5508.045789014619</v>
       </c>
       <c r="F11">
         <v>333897063436.1031</v>
@@ -4786,7 +4909,7 @@
         <v>2000</v>
       </c>
       <c r="B12">
-        <v>64.87725931834045</v>
+        <v>64.87725931834042</v>
       </c>
       <c r="C12">
         <v>240.0226281305118</v>
@@ -4795,10 +4918,10 @@
         <v>4.068546628759799</v>
       </c>
       <c r="E12">
-        <v>5473.200991268365</v>
+        <v>5473.200991268364</v>
       </c>
       <c r="F12">
-        <v>338377121313.0863</v>
+        <v>338377121313.0862</v>
       </c>
       <c r="G12">
         <v>23612.47577240211</v>
@@ -4853,10 +4976,10 @@
         <v>4.096193503837899</v>
       </c>
       <c r="E14">
-        <v>5348.614465491923</v>
+        <v>5348.614465491922</v>
       </c>
       <c r="F14">
-        <v>343747613367.1583</v>
+        <v>343747613367.1584</v>
       </c>
       <c r="G14">
         <v>24525.76897931392</v>
@@ -4888,7 +5011,7 @@
         <v>350768366703.1083</v>
       </c>
       <c r="G15">
-        <v>25334.48606797576</v>
+        <v>25334.48606797575</v>
       </c>
       <c r="H15">
         <v>1250196606073.298</v>
@@ -4902,7 +5025,7 @@
         <v>2004</v>
       </c>
       <c r="B16">
-        <v>65.06929697218474</v>
+        <v>65.06929697218476</v>
       </c>
       <c r="C16">
         <v>241.8269545103988</v>
@@ -4911,10 +5034,10 @@
         <v>3.881981873398027</v>
       </c>
       <c r="E16">
-        <v>5361.216989523544</v>
+        <v>5361.216989523545</v>
       </c>
       <c r="F16">
-        <v>361503349454.607</v>
+        <v>361503349454.6071</v>
       </c>
       <c r="G16">
         <v>26484.8646123765</v>
@@ -4931,19 +5054,19 @@
         <v>2005</v>
       </c>
       <c r="B17">
-        <v>65.135723602403</v>
+        <v>65.13572360240302</v>
       </c>
       <c r="C17">
         <v>242.3944387969077</v>
       </c>
       <c r="D17">
-        <v>4.319786137097334</v>
+        <v>4.319786137097335</v>
       </c>
       <c r="E17">
-        <v>5407.358318396236</v>
+        <v>5407.358318396237</v>
       </c>
       <c r="F17">
-        <v>372663965373.4004</v>
+        <v>372663965373.4005</v>
       </c>
       <c r="G17">
         <v>27617.89118573937</v>
@@ -4966,13 +5089,13 @@
         <v>243.0213485738719</v>
       </c>
       <c r="D18">
-        <v>4.538237228549127</v>
+        <v>4.538237228549128</v>
       </c>
       <c r="E18">
-        <v>5462.949868612265</v>
+        <v>5462.949868612267</v>
       </c>
       <c r="F18">
-        <v>385000071454.4874</v>
+        <v>385000071454.4875</v>
       </c>
       <c r="G18">
         <v>28790.06052991809</v>
@@ -4998,7 +5121,7 @@
         <v>4.683013453940997</v>
       </c>
       <c r="E19">
-        <v>5508.314333660424</v>
+        <v>5508.314333660423</v>
       </c>
       <c r="F19">
         <v>400011680336.61</v>
@@ -5024,13 +5147,13 @@
         <v>244.4452659647031</v>
       </c>
       <c r="D20">
-        <v>4.930288031250559</v>
+        <v>4.930288031250558</v>
       </c>
       <c r="E20">
-        <v>5556.971550509567</v>
+        <v>5556.971550509566</v>
       </c>
       <c r="F20">
-        <v>411758865334.8086</v>
+        <v>411758865334.8085</v>
       </c>
       <c r="G20">
         <v>31311.34869248958</v>
@@ -5056,7 +5179,7 @@
         <v>4.669715914993017</v>
       </c>
       <c r="E21">
-        <v>5620.640553348034</v>
+        <v>5620.640553348033</v>
       </c>
       <c r="F21">
         <v>414436748466.3683</v>
@@ -5076,7 +5199,7 @@
         <v>2010</v>
       </c>
       <c r="B22">
-        <v>65.39032864362724</v>
+        <v>65.39032864362723</v>
       </c>
       <c r="C22">
         <v>246.0478781116976</v>
@@ -5088,7 +5211,7 @@
         <v>5647.371233208592</v>
       </c>
       <c r="F22">
-        <v>417679449576.6617</v>
+        <v>417679449576.6616</v>
       </c>
       <c r="G22">
         <v>32229.09724349195</v>
@@ -5163,7 +5286,7 @@
         <v>2013</v>
       </c>
       <c r="B25">
-        <v>65.38192655660595</v>
+        <v>65.38192655660593</v>
       </c>
       <c r="C25">
         <v>248.6893764555158</v>
@@ -5175,7 +5298,7 @@
         <v>5729.421660492691</v>
       </c>
       <c r="F25">
-        <v>431599001609.4241</v>
+        <v>431599001609.424</v>
       </c>
       <c r="G25">
         <v>33863.10230300319</v>
@@ -5184,7 +5307,7 @@
         <v>1741269865576.235</v>
       </c>
       <c r="I25">
-        <v>9.505703634097443</v>
+        <v>9.505703634097442</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -5198,7 +5321,7 @@
         <v>249.6143639312732</v>
       </c>
       <c r="D26">
-        <v>3.986366838844056</v>
+        <v>3.986366838844055</v>
       </c>
       <c r="E26">
         <v>5741.799045766817</v>
@@ -5230,16 +5353,16 @@
         <v>3.866296940505554</v>
       </c>
       <c r="E27">
-        <v>5726.203238251433</v>
+        <v>5726.203238251434</v>
       </c>
       <c r="F27">
         <v>443261614618.7467</v>
       </c>
       <c r="G27">
-        <v>35095.93834326351</v>
+        <v>35095.9383432635</v>
       </c>
       <c r="H27">
-        <v>1818555746278.557</v>
+        <v>1818555746278.556</v>
       </c>
       <c r="I27">
         <v>9.213357502950581</v>
@@ -5262,7 +5385,7 @@
         <v>5716.045590815899</v>
       </c>
       <c r="F28">
-        <v>444976663139.318</v>
+        <v>444976663139.3179</v>
       </c>
       <c r="G28">
         <v>35400.55883589223</v>
@@ -5285,16 +5408,16 @@
         <v>252.5472942819621</v>
       </c>
       <c r="D29">
-        <v>4.268122654983457</v>
+        <v>4.268122654983456</v>
       </c>
       <c r="E29">
         <v>5725.285609447882</v>
       </c>
       <c r="F29">
-        <v>446654789434.985</v>
+        <v>446654789434.9849</v>
       </c>
       <c r="G29">
-        <v>35653.19290111172</v>
+        <v>35653.19290111171</v>
       </c>
       <c r="H29">
         <v>1859165372966.655</v>
@@ -5314,13 +5437,13 @@
         <v>253.5469568888901</v>
       </c>
       <c r="D30">
-        <v>4.036635944548346</v>
+        <v>4.036635944548347</v>
       </c>
       <c r="E30">
-        <v>5746.625354981675</v>
+        <v>5746.625354981677</v>
       </c>
       <c r="F30">
-        <v>449936898095.6995</v>
+        <v>449936898095.6996</v>
       </c>
       <c r="G30">
         <v>36013.77293253902</v>
@@ -5329,7 +5452,7 @@
         <v>1884304788720.434</v>
       </c>
       <c r="I30">
-        <v>8.846981668337641</v>
+        <v>8.846981668337643</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -5337,22 +5460,22 @@
         <v>2019</v>
       </c>
       <c r="B31">
-        <v>65.08471931750731</v>
+        <v>65.08471931750732</v>
       </c>
       <c r="C31">
-        <v>254.5465317906873</v>
+        <v>254.5465317906874</v>
       </c>
       <c r="D31">
-        <v>3.862431269321432</v>
+        <v>3.862431269321433</v>
       </c>
       <c r="E31">
-        <v>5751.226500749683</v>
+        <v>5751.226500749684</v>
       </c>
       <c r="F31">
-        <v>452915213813.0062</v>
+        <v>452915213813.0063</v>
       </c>
       <c r="G31">
-        <v>36324.28919096432</v>
+        <v>36324.28919096433</v>
       </c>
       <c r="H31">
         <v>1906593297746.301</v>
@@ -5466,25 +5589,25 @@
         <v>1980</v>
       </c>
       <c r="B2">
-        <v>57.1425581036766</v>
+        <v>57.14255810367661</v>
       </c>
       <c r="C2">
-        <v>235.0851566835621</v>
+        <v>235.0851566835622</v>
       </c>
       <c r="D2">
-        <v>0.04248482666874017</v>
+        <v>0.04248482666874018</v>
       </c>
       <c r="E2">
-        <v>366</v>
+        <v>366.0000000000001</v>
       </c>
       <c r="F2">
-        <v>47207847596.54369</v>
+        <v>47207847596.5437</v>
       </c>
       <c r="G2">
-        <v>266.577850783745</v>
+        <v>266.5778507837451</v>
       </c>
       <c r="H2">
-        <v>163030988939.2864</v>
+        <v>163030988939.2865</v>
       </c>
       <c r="I2">
         <v>16.75237579755089</v>
@@ -5495,13 +5618,13 @@
         <v>1981</v>
       </c>
       <c r="B3">
-        <v>57.16209944061295</v>
+        <v>57.16209944061296</v>
       </c>
       <c r="C3">
         <v>237.8906275648523</v>
       </c>
       <c r="D3">
-        <v>0.04503373764927773</v>
+        <v>0.04503373764927774</v>
       </c>
       <c r="E3">
         <v>389.0456821809645</v>
@@ -5510,7 +5633,7 @@
         <v>48882390749.51745</v>
       </c>
       <c r="G3">
-        <v>268.5538660827888</v>
+        <v>268.5538660827887</v>
       </c>
       <c r="H3">
         <v>164514851911.3914</v>
@@ -5524,7 +5647,7 @@
         <v>1982</v>
       </c>
       <c r="B4">
-        <v>57.18415732848981</v>
+        <v>57.18415732848982</v>
       </c>
       <c r="C4">
         <v>240.7729437474433</v>
@@ -5536,7 +5659,7 @@
         <v>396.2098965873458</v>
       </c>
       <c r="F4">
-        <v>50120574108.67735</v>
+        <v>50120574108.67736</v>
       </c>
       <c r="G4">
         <v>270.4630582872332</v>
@@ -5565,10 +5688,10 @@
         <v>413.3117302691283</v>
       </c>
       <c r="F5">
-        <v>52024520790.95903</v>
+        <v>52024520790.95902</v>
       </c>
       <c r="G5">
-        <v>275.8964714444836</v>
+        <v>275.8964714444837</v>
       </c>
       <c r="H5">
         <v>172080567138.984</v>
@@ -5582,19 +5705,19 @@
         <v>1984</v>
       </c>
       <c r="B6">
-        <v>57.24953222029595</v>
+        <v>57.24953222029594</v>
       </c>
       <c r="C6">
         <v>246.7390787329686</v>
       </c>
       <c r="D6">
-        <v>0.02682887327617561</v>
+        <v>0.0268288732761756</v>
       </c>
       <c r="E6">
         <v>441.3839402374289</v>
       </c>
       <c r="F6">
-        <v>53023649625.27629</v>
+        <v>53023649625.27628</v>
       </c>
       <c r="G6">
         <v>276.0603085282391</v>
@@ -5611,7 +5734,7 @@
         <v>1985</v>
       </c>
       <c r="B7">
-        <v>57.30195855660807</v>
+        <v>57.30195855660806</v>
       </c>
       <c r="C7">
         <v>249.8053639236519</v>
@@ -5623,7 +5746,7 @@
         <v>450.0620193730313</v>
       </c>
       <c r="F7">
-        <v>54620765830.69141</v>
+        <v>54620765830.6914</v>
       </c>
       <c r="G7">
         <v>279.7198462306384</v>
@@ -5649,7 +5772,7 @@
         <v>0.03287362177485117</v>
       </c>
       <c r="E8">
-        <v>464.0667044333523</v>
+        <v>464.0667044333524</v>
       </c>
       <c r="F8">
         <v>56485485382.25069</v>
@@ -5669,7 +5792,7 @@
         <v>1987</v>
       </c>
       <c r="B9">
-        <v>57.38471551873238</v>
+        <v>57.38471551873236</v>
       </c>
       <c r="C9">
         <v>256.0782038716675</v>
@@ -5681,7 +5804,7 @@
         <v>489.1942529751224</v>
       </c>
       <c r="F9">
-        <v>58984509386.61477</v>
+        <v>58984509386.61476</v>
       </c>
       <c r="G9">
         <v>292.2772445124663</v>
@@ -5698,22 +5821,22 @@
         <v>1988</v>
       </c>
       <c r="B10">
-        <v>57.43902251617995</v>
+        <v>57.43902251617996</v>
       </c>
       <c r="C10">
-        <v>259.2807034711461</v>
+        <v>259.2807034711462</v>
       </c>
       <c r="D10">
-        <v>0.03785515650528552</v>
+        <v>0.03785515650528553</v>
       </c>
       <c r="E10">
-        <v>508.8513946302882</v>
+        <v>508.8513946302884</v>
       </c>
       <c r="F10">
-        <v>61516835938.70349</v>
+        <v>61516835938.70351</v>
       </c>
       <c r="G10">
-        <v>300.0186980186716</v>
+        <v>300.0186980186717</v>
       </c>
       <c r="H10">
         <v>196333899574.5557</v>
@@ -5727,19 +5850,19 @@
         <v>1989</v>
       </c>
       <c r="B11">
-        <v>57.5048308500369</v>
+        <v>57.50483085003691</v>
       </c>
       <c r="C11">
         <v>262.5256829465416</v>
       </c>
       <c r="D11">
-        <v>0.04325948897242089</v>
+        <v>0.0432594889724209</v>
       </c>
       <c r="E11">
         <v>528.47413211846</v>
       </c>
       <c r="F11">
-        <v>63807119552.54668</v>
+        <v>63807119552.54669</v>
       </c>
       <c r="G11">
         <v>305.2850833023268</v>
@@ -5785,7 +5908,7 @@
         <v>1991</v>
       </c>
       <c r="B13">
-        <v>57.65892079214418</v>
+        <v>57.65892079214419</v>
       </c>
       <c r="C13">
         <v>269.1399566751585</v>
@@ -5814,13 +5937,13 @@
         <v>1992</v>
       </c>
       <c r="B14">
-        <v>57.7404274538283</v>
+        <v>57.74042745382831</v>
       </c>
       <c r="C14">
-        <v>272.5067982124134</v>
+        <v>272.5067982124135</v>
       </c>
       <c r="D14">
-        <v>0.04929747007496117</v>
+        <v>0.04929747007496118</v>
       </c>
       <c r="E14">
         <v>527.840527481397</v>
@@ -5849,10 +5972,10 @@
         <v>275.912859876338</v>
       </c>
       <c r="D15">
-        <v>0.06206597232652195</v>
+        <v>0.06206597232652194</v>
       </c>
       <c r="E15">
-        <v>514.4082023137875</v>
+        <v>514.4082023137873</v>
       </c>
       <c r="F15">
         <v>68417842378.57166</v>
@@ -5872,7 +5995,7 @@
         <v>1994</v>
       </c>
       <c r="B16">
-        <v>57.92503769418602</v>
+        <v>57.92503769418601</v>
       </c>
       <c r="C16">
         <v>279.3590871986133</v>
@@ -5884,7 +6007,7 @@
         <v>518.4320822949929</v>
       </c>
       <c r="F16">
-        <v>70217644899.04509</v>
+        <v>70217644899.0451</v>
       </c>
       <c r="G16">
         <v>313.5377510785804</v>
@@ -5901,7 +6024,7 @@
         <v>1995</v>
       </c>
       <c r="B17">
-        <v>58.03325954868893</v>
+        <v>58.03325954868895</v>
       </c>
       <c r="C17">
         <v>282.8468002347069</v>
@@ -5930,7 +6053,7 @@
         <v>1996</v>
       </c>
       <c r="B18">
-        <v>58.14695913679319</v>
+        <v>58.1469591367932</v>
       </c>
       <c r="C18">
         <v>286.3770396026165</v>
@@ -5942,10 +6065,10 @@
         <v>531.6421235796695</v>
       </c>
       <c r="F18">
-        <v>75508917124.25673</v>
+        <v>75508917124.25676</v>
       </c>
       <c r="G18">
-        <v>324.2881363468034</v>
+        <v>324.2881363468035</v>
       </c>
       <c r="H18">
         <v>221723173005.6702</v>
@@ -5988,7 +6111,7 @@
         <v>1998</v>
       </c>
       <c r="B20">
-        <v>58.39944740935875</v>
+        <v>58.39944740935874</v>
       </c>
       <c r="C20">
         <v>293.5646818413273</v>
@@ -5997,7 +6120,7 @@
         <v>0.23649401983097</v>
       </c>
       <c r="E20">
-        <v>531.3775508979041</v>
+        <v>531.377550897904</v>
       </c>
       <c r="F20">
         <v>80874215707.46373</v>
@@ -6029,7 +6152,7 @@
         <v>531.3658759862836</v>
       </c>
       <c r="F21">
-        <v>83557329084.832</v>
+        <v>83557329084.83202</v>
       </c>
       <c r="G21">
         <v>343.3497042034654</v>
@@ -6055,13 +6178,13 @@
         <v>0.2846053644865145</v>
       </c>
       <c r="E22">
-        <v>532.3998729609697</v>
+        <v>532.3998729609698</v>
       </c>
       <c r="F22">
-        <v>86378512260.61057</v>
+        <v>86378512260.61055</v>
       </c>
       <c r="G22">
-        <v>349.6963941674796</v>
+        <v>349.6963941674795</v>
       </c>
       <c r="H22">
         <v>249050818314.9629</v>
@@ -6075,7 +6198,7 @@
         <v>2001</v>
       </c>
       <c r="B23">
-        <v>58.84404488529803</v>
+        <v>58.84404488529804</v>
       </c>
       <c r="C23">
         <v>304.6371525291345</v>
@@ -6104,10 +6227,10 @@
         <v>2002</v>
       </c>
       <c r="B24">
-        <v>59.00219697728448</v>
+        <v>59.00219697728447</v>
       </c>
       <c r="C24">
-        <v>308.3946838957296</v>
+        <v>308.3946838957297</v>
       </c>
       <c r="D24">
         <v>0.3724913075693834</v>
@@ -6142,16 +6265,16 @@
         <v>0.3859933726403315</v>
       </c>
       <c r="E25">
-        <v>535.0001507582934</v>
+        <v>535.0001507582933</v>
       </c>
       <c r="F25">
         <v>96482947172.4511</v>
       </c>
       <c r="G25">
-        <v>373.4459832448332</v>
+        <v>373.4459832448331</v>
       </c>
       <c r="H25">
-        <v>274096514772.5242</v>
+        <v>274096514772.5243</v>
       </c>
       <c r="I25">
         <v>15.58738664870186</v>
@@ -6162,16 +6285,16 @@
         <v>2004</v>
       </c>
       <c r="B26">
-        <v>59.33513549596041</v>
+        <v>59.3351354959604</v>
       </c>
       <c r="C26">
-        <v>315.9946352385636</v>
+        <v>315.9946352385637</v>
       </c>
       <c r="D26">
-        <v>0.4073586644384107</v>
+        <v>0.4073586644384106</v>
       </c>
       <c r="E26">
-        <v>544.7637502132401</v>
+        <v>544.7637502132402</v>
       </c>
       <c r="F26">
         <v>102714766505.7288</v>
@@ -6206,10 +6329,10 @@
         <v>110369208239.6911</v>
       </c>
       <c r="G27">
-        <v>405.6987975141775</v>
+        <v>405.6987975141776</v>
       </c>
       <c r="H27">
-        <v>300900273413.7456</v>
+        <v>300900273413.7455</v>
       </c>
       <c r="I27">
         <v>15.97301704470109</v>
@@ -6220,7 +6343,7 @@
         <v>2006</v>
       </c>
       <c r="B28">
-        <v>59.68645655809463</v>
+        <v>59.68645655809464</v>
       </c>
       <c r="C28">
         <v>323.6947573940918</v>
@@ -6255,7 +6378,7 @@
         <v>327.5775150393904</v>
       </c>
       <c r="D29">
-        <v>0.6053847693495892</v>
+        <v>0.6053847693495893</v>
       </c>
       <c r="E29">
         <v>593.255795444938</v>
@@ -6264,7 +6387,7 @@
         <v>133407836797.4286</v>
       </c>
       <c r="G29">
-        <v>458.5909395195473</v>
+        <v>458.5909395195472</v>
       </c>
       <c r="H29">
         <v>343083736914.037</v>
@@ -6278,13 +6401,13 @@
         <v>2008</v>
       </c>
       <c r="B30">
-        <v>60.04632218424055</v>
+        <v>60.04632218424056</v>
       </c>
       <c r="C30">
         <v>331.4774059924256</v>
       </c>
       <c r="D30">
-        <v>0.7595878983686041</v>
+        <v>0.759587898368604</v>
       </c>
       <c r="E30">
         <v>626.0221481038664</v>
@@ -6293,10 +6416,10 @@
         <v>145676473240.885</v>
       </c>
       <c r="G30">
-        <v>486.204645998844</v>
+        <v>486.2046459988439</v>
       </c>
       <c r="H30">
-        <v>366750538808.1126</v>
+        <v>366750538808.1127</v>
       </c>
       <c r="I30">
         <v>17.09867414895781</v>
@@ -6345,7 +6468,7 @@
         <v>0.8926773635941145</v>
       </c>
       <c r="E32">
-        <v>704.3728842780333</v>
+        <v>704.3728842780332</v>
       </c>
       <c r="F32">
         <v>176752379008.8003</v>
@@ -6365,22 +6488,22 @@
         <v>2011</v>
       </c>
       <c r="B33">
-        <v>60.61483778053876</v>
+        <v>60.61483778053875</v>
       </c>
       <c r="C33">
         <v>343.2168803202094</v>
       </c>
       <c r="D33">
-        <v>0.946125330871597</v>
+        <v>0.9461253308715969</v>
       </c>
       <c r="E33">
-        <v>752.4702950781234</v>
+        <v>752.4702950781235</v>
       </c>
       <c r="F33">
         <v>194728031480.6451</v>
       </c>
       <c r="G33">
-        <v>601.662095317902</v>
+        <v>601.6620953179021</v>
       </c>
       <c r="H33">
         <v>466902416464.9962</v>
@@ -6429,10 +6552,10 @@
         <v>351.013238023661</v>
       </c>
       <c r="D35">
-        <v>0.9891936017545859</v>
+        <v>0.9891936017545857</v>
       </c>
       <c r="E35">
-        <v>835.4131883048892</v>
+        <v>835.4131883048891</v>
       </c>
       <c r="F35">
         <v>225657075126.965</v>
@@ -6441,7 +6564,7 @@
         <v>679.1004430407532</v>
       </c>
       <c r="H35">
-        <v>538160374608.3877</v>
+        <v>538160374608.3876</v>
       </c>
       <c r="I35">
         <v>15.25302269276287</v>
@@ -6499,7 +6622,7 @@
         <v>759.9347303660041</v>
       </c>
       <c r="H37">
-        <v>617295052424.6954</v>
+        <v>617295052424.6953</v>
       </c>
       <c r="I37">
         <v>15.58385458634904</v>
@@ -6510,7 +6633,7 @@
         <v>2016</v>
       </c>
       <c r="B38">
-        <v>61.65411350422362</v>
+        <v>61.65411350422361</v>
       </c>
       <c r="C38">
         <v>362.6035606817686</v>
@@ -6519,13 +6642,13 @@
         <v>1.108250301122617</v>
       </c>
       <c r="E38">
-        <v>967.7883175233152</v>
+        <v>967.7883175233151</v>
       </c>
       <c r="F38">
         <v>271927885736.443</v>
       </c>
       <c r="G38">
-        <v>803.0987544132573</v>
+        <v>803.0987544132572</v>
       </c>
       <c r="H38">
         <v>660785383243.0421</v>
@@ -6539,10 +6662,10 @@
         <v>2017</v>
       </c>
       <c r="B39">
-        <v>61.86779200890481</v>
+        <v>61.86779200890479</v>
       </c>
       <c r="C39">
-        <v>366.4380678042616</v>
+        <v>366.4380678042617</v>
       </c>
       <c r="D39">
         <v>1.125709474103168</v>
@@ -6557,7 +6680,7 @@
         <v>854.6174346030417</v>
       </c>
       <c r="H39">
-        <v>712488565088.8245</v>
+        <v>712488565088.8243</v>
       </c>
       <c r="I39">
         <v>15.01823875014704</v>
@@ -6568,10 +6691,10 @@
         <v>2018</v>
       </c>
       <c r="B40">
-        <v>62.07921430913986</v>
+        <v>62.07921430913987</v>
       </c>
       <c r="C40">
-        <v>370.2577939196144</v>
+        <v>370.2577939196145</v>
       </c>
       <c r="D40">
         <v>1.144374955555147</v>
@@ -6580,13 +6703,13 @@
         <v>1102.968171972239</v>
       </c>
       <c r="F40">
-        <v>309032416772.6615</v>
+        <v>309032416772.6616</v>
       </c>
       <c r="G40">
-        <v>903.9731786730874</v>
+        <v>903.9731786730875</v>
       </c>
       <c r="H40">
-        <v>763524634131.5629</v>
+        <v>763524634131.563</v>
       </c>
       <c r="I40">
         <v>14.88153066744756</v>
@@ -6597,10 +6720,10 @@
         <v>2019</v>
       </c>
       <c r="B41">
-        <v>62.2889835609348</v>
+        <v>62.28898356093482</v>
       </c>
       <c r="C41">
-        <v>374.0625700230933</v>
+        <v>374.0625700230934</v>
       </c>
       <c r="D41">
         <v>1.171764619120355</v>
@@ -6612,10 +6735,10 @@
         <v>325535436467.8896</v>
       </c>
       <c r="G41">
-        <v>953.7371471951138</v>
+        <v>953.7371471951141</v>
       </c>
       <c r="H41">
-        <v>817747431055.3933</v>
+        <v>817747431055.3934</v>
       </c>
       <c r="I41">
         <v>13.47361810745156</v>
@@ -6626,7 +6749,7 @@
         <v>2020</v>
       </c>
       <c r="B42">
-        <v>62.49832744176252</v>
+        <v>62.49832744176253</v>
       </c>
       <c r="C42">
         <v>377.8521946346955</v>
@@ -6686,7 +6809,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6735,28 +6858,28 @@
         <v>39.8400001525879</v>
       </c>
       <c r="C2">
-        <v>69.5928714312201</v>
+        <v>69.59287143122012</v>
       </c>
       <c r="D2">
-        <v>343.3296763576522</v>
+        <v>343.3296763576523</v>
       </c>
       <c r="E2">
         <v>0.01777196340516677</v>
       </c>
       <c r="F2">
-        <v>6007.8999023438</v>
+        <v>6007.899902343801</v>
       </c>
       <c r="G2">
         <v>1727278152939.404</v>
       </c>
       <c r="H2">
-        <v>39933.51505648736</v>
+        <v>39933.51505648737</v>
       </c>
       <c r="I2">
-        <v>3373095791123.574</v>
+        <v>3373095791123.575</v>
       </c>
       <c r="J2">
-        <v>34.189998626709</v>
+        <v>34.18999862670901</v>
       </c>
       <c r="K2">
         <v>23.46921539563932</v>
@@ -6767,19 +6890,19 @@
         <v>1995</v>
       </c>
       <c r="B3">
-        <v>39.65865379293966</v>
+        <v>39.65865379293967</v>
       </c>
       <c r="C3">
-        <v>69.5221067094301</v>
+        <v>69.52210670943012</v>
       </c>
       <c r="D3">
         <v>343.7474810922041</v>
       </c>
       <c r="E3">
-        <v>0.008951091192708495</v>
+        <v>0.008951091192708496</v>
       </c>
       <c r="F3">
-        <v>6282.563165378101</v>
+        <v>6282.563165378102</v>
       </c>
       <c r="G3">
         <v>1818346571127.991</v>
@@ -6805,16 +6928,16 @@
         <v>39.54464125569261</v>
       </c>
       <c r="C4">
-        <v>69.43223176639869</v>
+        <v>69.4322317663987</v>
       </c>
       <c r="D4">
-        <v>344.2000427533756</v>
+        <v>344.2000427533757</v>
       </c>
       <c r="E4">
-        <v>0.005470804901520293</v>
+        <v>0.005470804901520294</v>
       </c>
       <c r="F4">
-        <v>6468.164310073582</v>
+        <v>6468.164310073583</v>
       </c>
       <c r="G4">
         <v>1771720721529.503</v>
@@ -6823,10 +6946,10 @@
         <v>41072.06789776314</v>
       </c>
       <c r="I4">
-        <v>3486097338022.665</v>
+        <v>3486097338022.666</v>
       </c>
       <c r="J4">
-        <v>33.75502909833989</v>
+        <v>33.7550290983399</v>
       </c>
       <c r="K4">
         <v>23.36115643732072</v>
@@ -6843,13 +6966,13 @@
         <v>69.32399993894688</v>
       </c>
       <c r="D5">
-        <v>344.6543999146249</v>
+        <v>344.6543999146248</v>
       </c>
       <c r="E5">
         <v>0.0193312527644669</v>
       </c>
       <c r="F5">
-        <v>6756.12257134326</v>
+        <v>6756.122571343259</v>
       </c>
       <c r="G5">
         <v>1702958970601.498</v>
@@ -6861,7 +6984,7 @@
         <v>3365109518174.461</v>
       </c>
       <c r="J5">
-        <v>33.61749216313168</v>
+        <v>33.61749216313167</v>
       </c>
       <c r="K5">
         <v>23.35048737419174</v>
@@ -6872,10 +6995,10 @@
         <v>1998</v>
       </c>
       <c r="B6">
-        <v>39.30806770149255</v>
+        <v>39.30806770149254</v>
       </c>
       <c r="C6">
-        <v>69.20035595318372</v>
+        <v>69.2003559531837</v>
       </c>
       <c r="D6">
         <v>345.1425193733887</v>
@@ -6884,19 +7007,19 @@
         <v>0.0289836725442736</v>
       </c>
       <c r="F6">
-        <v>6930.478138101795</v>
+        <v>6930.478138101793</v>
       </c>
       <c r="G6">
         <v>1625888596162.927</v>
       </c>
       <c r="H6">
-        <v>37920.28372990449</v>
+        <v>37920.28372990448</v>
       </c>
       <c r="I6">
         <v>3238369275739.513</v>
       </c>
       <c r="J6">
-        <v>33.2960310157382</v>
+        <v>33.29603101573819</v>
       </c>
       <c r="K6">
         <v>22.83664375633507</v>
@@ -6907,25 +7030,25 @@
         <v>1999</v>
       </c>
       <c r="B7">
-        <v>39.14188350234356</v>
+        <v>39.14188350234355</v>
       </c>
       <c r="C7">
         <v>69.06446515487558</v>
       </c>
       <c r="D7">
-        <v>345.5921788412979</v>
+        <v>345.5921788412978</v>
       </c>
       <c r="E7">
         <v>0.08645700596583604</v>
       </c>
       <c r="F7">
-        <v>7187.293950973181</v>
+        <v>7187.293950973182</v>
       </c>
       <c r="G7">
         <v>1605675632169.079</v>
       </c>
       <c r="H7">
-        <v>37660.49469670721</v>
+        <v>37660.4946967072</v>
       </c>
       <c r="I7">
         <v>3242608976661.524</v>
@@ -6963,13 +7086,13 @@
         <v>37925.67363722395</v>
       </c>
       <c r="I8">
-        <v>3285855224095.285</v>
+        <v>3285855224095.286</v>
       </c>
       <c r="J8">
         <v>32.73161164205116</v>
       </c>
       <c r="K8">
-        <v>22.45220880818845</v>
+        <v>22.45220880818844</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -6989,7 +7112,7 @@
         <v>0.1096314590402939</v>
       </c>
       <c r="F9">
-        <v>7474.598278542595</v>
+        <v>7474.598278542594</v>
       </c>
       <c r="G9">
         <v>1567323400534.798</v>
@@ -6998,7 +7121,7 @@
         <v>37366.28624690825</v>
       </c>
       <c r="I9">
-        <v>3261803115264.882</v>
+        <v>3261803115264.881</v>
       </c>
       <c r="J9">
         <v>32.40870771878301</v>
@@ -7024,7 +7147,7 @@
         <v>0.1339587159172803</v>
       </c>
       <c r="F10">
-        <v>7581.158477682459</v>
+        <v>7581.158477682461</v>
       </c>
       <c r="G10">
         <v>1523074880563.888</v>
@@ -7033,7 +7156,7 @@
         <v>36702.83371294747</v>
       </c>
       <c r="I10">
-        <v>3230403391241.764</v>
+        <v>3230403391241.765</v>
       </c>
       <c r="J10">
         <v>32.0483793275274</v>
@@ -7047,19 +7170,19 @@
         <v>2003</v>
       </c>
       <c r="B11">
-        <v>38.16088405887349</v>
+        <v>38.1608840588735</v>
       </c>
       <c r="C11">
-        <v>68.41236638537302</v>
+        <v>68.41236638537303</v>
       </c>
       <c r="D11">
-        <v>347.3962921394136</v>
+        <v>347.3962921394137</v>
       </c>
       <c r="E11">
         <v>0.1421143354911683</v>
       </c>
       <c r="F11">
-        <v>7675.901792189728</v>
+        <v>7675.901792189729</v>
       </c>
       <c r="G11">
         <v>1500876482754.368</v>
@@ -7071,7 +7194,7 @@
         <v>3238113357428.486</v>
       </c>
       <c r="J11">
-        <v>31.65520176316763</v>
+        <v>31.65520176316764</v>
       </c>
       <c r="K11">
         <v>20.91713129374546</v>
@@ -7085,7 +7208,7 @@
         <v>37.82852705585948</v>
       </c>
       <c r="C12">
-        <v>68.22297996678346</v>
+        <v>68.22297996678344</v>
       </c>
       <c r="D12">
         <v>347.79269352214</v>
@@ -7094,7 +7217,7 @@
         <v>0.143607958520565</v>
       </c>
       <c r="F12">
-        <v>7807.315541048415</v>
+        <v>7807.315541048413</v>
       </c>
       <c r="G12">
         <v>1496477133503.05</v>
@@ -7123,13 +7246,13 @@
         <v>68.01767529038435</v>
       </c>
       <c r="D13">
-        <v>348.1238509330294</v>
+        <v>348.1238509330295</v>
       </c>
       <c r="E13">
         <v>0.1399229642593562</v>
       </c>
       <c r="F13">
-        <v>7896.642082832467</v>
+        <v>7896.642082832466</v>
       </c>
       <c r="G13">
         <v>1490067676847.499</v>
@@ -7164,7 +7287,7 @@
         <v>0.1179143826728049</v>
       </c>
       <c r="F14">
-        <v>7963.510218112395</v>
+        <v>7963.510218112394</v>
       </c>
       <c r="G14">
         <v>1475744798282.418</v>
@@ -7176,7 +7299,7 @@
         <v>3308911296020.755</v>
       </c>
       <c r="J14">
-        <v>30.49493181041081</v>
+        <v>30.49493181041082</v>
       </c>
       <c r="K14">
         <v>21.3992856851895</v>
@@ -7190,10 +7313,10 @@
         <v>36.99158260707625</v>
       </c>
       <c r="C15">
-        <v>67.57299566528675</v>
+        <v>67.57299566528674</v>
       </c>
       <c r="D15">
-        <v>348.7275101674464</v>
+        <v>348.7275101674463</v>
       </c>
       <c r="E15">
         <v>0.1568019888369709</v>
@@ -7205,10 +7328,10 @@
         <v>1462548958524.879</v>
       </c>
       <c r="H15">
-        <v>36667.10412986288</v>
+        <v>36667.10412986287</v>
       </c>
       <c r="I15">
-        <v>3310010300889.384</v>
+        <v>3310010300889.383</v>
       </c>
       <c r="J15">
         <v>30.16631164498811</v>
@@ -7228,13 +7351,13 @@
         <v>67.32800948868697</v>
       </c>
       <c r="D16">
-        <v>349.0030897648645</v>
+        <v>349.0030897648646</v>
       </c>
       <c r="E16">
         <v>0.1911431491683784</v>
       </c>
       <c r="F16">
-        <v>8031.879448280977</v>
+        <v>8031.879448280978</v>
       </c>
       <c r="G16">
         <v>1463319908063.358</v>
@@ -7257,10 +7380,10 @@
         <v>2009</v>
       </c>
       <c r="B17">
-        <v>36.46609905828574</v>
+        <v>36.46609905828575</v>
       </c>
       <c r="C17">
-        <v>67.06340980242105</v>
+        <v>67.06340980242106</v>
       </c>
       <c r="D17">
         <v>349.2366548587956</v>
@@ -7292,10 +7415,10 @@
         <v>2010</v>
       </c>
       <c r="B18">
-        <v>36.15637741489113</v>
+        <v>36.15637741489114</v>
       </c>
       <c r="C18">
-        <v>66.77539904411186</v>
+        <v>66.77539904411188</v>
       </c>
       <c r="D18">
         <v>349.4461618042703</v>
@@ -7304,7 +7427,7 @@
         <v>0.1887002500237362</v>
       </c>
       <c r="F18">
-        <v>8224.357068779876</v>
+        <v>8224.357068779878</v>
       </c>
       <c r="G18">
         <v>1477279066402.075</v>
@@ -7345,7 +7468,7 @@
         <v>1495236758666.001</v>
       </c>
       <c r="H19">
-        <v>39202.35511579172</v>
+        <v>39202.35511579171</v>
       </c>
       <c r="I19">
         <v>3647741525156.167</v>
@@ -7365,7 +7488,7 @@
         <v>35.61808786119032</v>
       </c>
       <c r="C20">
-        <v>66.12897380119071</v>
+        <v>66.12897380119072</v>
       </c>
       <c r="D20">
         <v>349.6216298115082</v>
@@ -7380,7 +7503,7 @@
         <v>1511224345614.367</v>
       </c>
       <c r="H20">
-        <v>40132.68078864972</v>
+        <v>40132.68078864973</v>
       </c>
       <c r="I20">
         <v>3762070413554.62</v>
@@ -7409,7 +7532,7 @@
         <v>0.1588267454805303</v>
       </c>
       <c r="F21">
-        <v>7944.985994153089</v>
+        <v>7944.98599415309</v>
       </c>
       <c r="G21">
         <v>1500062896894.875</v>
@@ -7485,7 +7608,7 @@
         <v>1466645358991.635</v>
       </c>
       <c r="H23">
-        <v>39601.51120058032</v>
+        <v>39601.51120058031</v>
       </c>
       <c r="I23">
         <v>3751933505491.584</v>
@@ -7502,10 +7625,10 @@
         <v>2016</v>
       </c>
       <c r="B24">
-        <v>34.79576310667117</v>
+        <v>34.79576310667116</v>
       </c>
       <c r="C24">
-        <v>64.6186602740412</v>
+        <v>64.61866027404119</v>
       </c>
       <c r="D24">
         <v>349.4395696213123</v>
@@ -7514,7 +7637,7 @@
         <v>0.2307018698796639</v>
       </c>
       <c r="F24">
-        <v>8178.072794865572</v>
+        <v>8178.07279486557</v>
       </c>
       <c r="G24">
         <v>1463704637577.467</v>
@@ -7537,7 +7660,7 @@
         <v>2017</v>
       </c>
       <c r="B25">
-        <v>34.62043883718835</v>
+        <v>34.62043883718836</v>
       </c>
       <c r="C25">
         <v>64.2331293297043</v>
@@ -7546,22 +7669,22 @@
         <v>349.3467295813325</v>
       </c>
       <c r="E25">
-        <v>0.2434850124558393</v>
+        <v>0.2434850124558394</v>
       </c>
       <c r="F25">
-        <v>8390.803090003785</v>
+        <v>8390.803090003787</v>
       </c>
       <c r="G25">
         <v>1460347193895.25</v>
       </c>
       <c r="H25">
-        <v>39518.5346586015</v>
+        <v>39518.53465860151</v>
       </c>
       <c r="I25">
-        <v>3740821282711.972</v>
+        <v>3740821282711.974</v>
       </c>
       <c r="J25">
-        <v>27.1132727515633</v>
+        <v>27.11327275156331</v>
       </c>
       <c r="K25">
         <v>20.43594606860216</v>
@@ -7578,10 +7701,10 @@
         <v>63.85627358700645</v>
       </c>
       <c r="D26">
-        <v>349.2260755188531</v>
+        <v>349.2260755188532</v>
       </c>
       <c r="E26">
-        <v>0.2651030997308148</v>
+        <v>0.2651030997308149</v>
       </c>
       <c r="F26">
         <v>8476.927621355208</v>
@@ -7593,7 +7716,7 @@
         <v>39535.97789676898</v>
       </c>
       <c r="I26">
-        <v>3741371126232.943</v>
+        <v>3741371126232.944</v>
       </c>
       <c r="J26">
         <v>26.88887671742862</v>
@@ -7610,7 +7733,7 @@
         <v>34.27278216686763</v>
       </c>
       <c r="C27">
-        <v>63.49067176699594</v>
+        <v>63.49067176699593</v>
       </c>
       <c r="D27">
         <v>349.0767082329424</v>
@@ -7670,6 +7793,41 @@
       </c>
       <c r="K28">
         <v>19.74777174028171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>2021</v>
+      </c>
+      <c r="B29">
+        <v>34.65434836528686</v>
+      </c>
+      <c r="C29">
+        <v>62.79689866099226</v>
+      </c>
+      <c r="D29">
+        <v>348.5188590971177</v>
+      </c>
+      <c r="E29">
+        <v>0.5060704875307959</v>
+      </c>
+      <c r="F29">
+        <v>8212.407272147704</v>
+      </c>
+      <c r="G29">
+        <v>1461409618601.227</v>
+      </c>
+      <c r="H29">
+        <v>39507.2893393063</v>
+      </c>
+      <c r="I29">
+        <v>3738923198132.295</v>
+      </c>
+      <c r="J29">
+        <v>27.16158167737659</v>
+      </c>
+      <c r="K29">
+        <v>21.14416625737088</v>
       </c>
     </row>
   </sheetData>
@@ -7719,7 +7877,7 @@
         <v>1980</v>
       </c>
       <c r="B2">
-        <v>68.2333286892832</v>
+        <v>68.23332868928321</v>
       </c>
       <c r="C2">
         <v>3602.902985074627</v>
@@ -7728,13 +7886,13 @@
         <v>10.38772838052267</v>
       </c>
       <c r="E2">
-        <v>544.0999755859</v>
+        <v>544.0999755859001</v>
       </c>
       <c r="F2">
-        <v>4149452772.923756</v>
+        <v>4149452772.923757</v>
       </c>
       <c r="G2">
-        <v>4928.13911785754</v>
+        <v>4928.139117857541</v>
       </c>
       <c r="H2">
         <v>7155338912.903522</v>
@@ -7757,13 +7915,13 @@
         <v>11.05235819235241</v>
       </c>
       <c r="E3">
-        <v>594.9040140889653</v>
+        <v>594.9040140889654</v>
       </c>
       <c r="F3">
-        <v>4516830414.591758</v>
+        <v>4516830414.591759</v>
       </c>
       <c r="G3">
-        <v>5264.042062266155</v>
+        <v>5264.042062266156</v>
       </c>
       <c r="H3">
         <v>7642148150.500759</v>
@@ -7777,16 +7935,16 @@
         <v>1982</v>
       </c>
       <c r="B4">
-        <v>68.92792110672615</v>
+        <v>68.92792110672616</v>
       </c>
       <c r="C4">
-        <v>3778.896908591952</v>
+        <v>3778.896908591953</v>
       </c>
       <c r="D4">
         <v>10.68427786189904</v>
       </c>
       <c r="E4">
-        <v>642.6788276319553</v>
+        <v>642.6788276319554</v>
       </c>
       <c r="F4">
         <v>4801310449.633166</v>
@@ -7795,7 +7953,7 @@
         <v>5537.969599535328</v>
       </c>
       <c r="H4">
-        <v>8126939769.139263</v>
+        <v>8126939769.139264</v>
       </c>
       <c r="I4">
         <v>22.29291490588914</v>
@@ -7806,7 +7964,7 @@
         <v>1983</v>
       </c>
       <c r="B5">
-        <v>69.15102245926134</v>
+        <v>69.15102245926133</v>
       </c>
       <c r="C5">
         <v>3835.410645778871</v>
@@ -7815,16 +7973,16 @@
         <v>9.590904168434047</v>
       </c>
       <c r="E5">
-        <v>694.2779607065613</v>
+        <v>694.2779607065612</v>
       </c>
       <c r="F5">
         <v>5136882477.03647</v>
       </c>
       <c r="G5">
-        <v>5815.928017992337</v>
+        <v>5815.928017992336</v>
       </c>
       <c r="H5">
-        <v>8521053860.863684</v>
+        <v>8521053860.863685</v>
       </c>
       <c r="I5">
         <v>21.46434389615849</v>
@@ -7838,25 +7996,25 @@
         <v>69.34160899586493</v>
       </c>
       <c r="C6">
-        <v>3884.896749064233</v>
+        <v>3884.896749064232</v>
       </c>
       <c r="D6">
-        <v>8.979000375248287</v>
+        <v>8.979000375248283</v>
       </c>
       <c r="E6">
         <v>748.7407893680495</v>
       </c>
       <c r="F6">
-        <v>5505513236.670382</v>
+        <v>5505513236.67038</v>
       </c>
       <c r="G6">
-        <v>6104.112266952456</v>
+        <v>6104.112266952455</v>
       </c>
       <c r="H6">
-        <v>8964410443.943081</v>
+        <v>8964410443.943079</v>
       </c>
       <c r="I6">
-        <v>21.40238291509307</v>
+        <v>21.40238291509306</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -7864,7 +8022,7 @@
         <v>1985</v>
       </c>
       <c r="B7">
-        <v>69.53013090614469</v>
+        <v>69.53013090614468</v>
       </c>
       <c r="C7">
         <v>3918.837567325126</v>
@@ -7876,13 +8034,13 @@
         <v>788.4297510203063</v>
       </c>
       <c r="F7">
-        <v>5617914454.501232</v>
+        <v>5617914454.501233</v>
       </c>
       <c r="G7">
-        <v>6257.505426977814</v>
+        <v>6257.505426977813</v>
       </c>
       <c r="H7">
-        <v>9335976945.116425</v>
+        <v>9335976945.116423</v>
       </c>
       <c r="I7">
         <v>20.11536164922619</v>
@@ -7902,7 +8060,7 @@
         <v>8.499562314624752</v>
       </c>
       <c r="E8">
-        <v>836.029950306683</v>
+        <v>836.0299503066831</v>
       </c>
       <c r="F8">
         <v>5697347236.238876</v>
@@ -7911,7 +8069,7 @@
         <v>6337.350531006057</v>
       </c>
       <c r="H8">
-        <v>9582861888.550417</v>
+        <v>9582861888.550415</v>
       </c>
       <c r="I8">
         <v>22.61381615789615</v>
@@ -7928,10 +8086,10 @@
         <v>3968.265103684977</v>
       </c>
       <c r="D9">
-        <v>9.154317383100679</v>
+        <v>9.154317383100677</v>
       </c>
       <c r="E9">
-        <v>890.4948307968434</v>
+        <v>890.4948307968433</v>
       </c>
       <c r="F9">
         <v>5843094398.574159</v>
@@ -7940,7 +8098,7 @@
         <v>6492.896970466735</v>
       </c>
       <c r="H9">
-        <v>9930390474.889807</v>
+        <v>9930390474.889805</v>
       </c>
       <c r="I9">
         <v>24.09005587328071</v>
@@ -7954,13 +8112,13 @@
         <v>70.19856889806029</v>
       </c>
       <c r="C10">
-        <v>4000.601873299452</v>
+        <v>4000.601873299453</v>
       </c>
       <c r="D10">
-        <v>9.761469914531951</v>
+        <v>9.761469914531952</v>
       </c>
       <c r="E10">
-        <v>949.2123442033692</v>
+        <v>949.2123442033694</v>
       </c>
       <c r="F10">
         <v>6152656817.338311</v>
@@ -7980,19 +8138,19 @@
         <v>1989</v>
       </c>
       <c r="B11">
-        <v>70.44896491686936</v>
+        <v>70.44896491686937</v>
       </c>
       <c r="C11">
-        <v>4039.703038819681</v>
+        <v>4039.703038819682</v>
       </c>
       <c r="D11">
-        <v>9.731509592298121</v>
+        <v>9.731509592298123</v>
       </c>
       <c r="E11">
         <v>1021.467377079909</v>
       </c>
       <c r="F11">
-        <v>6532567220.038189</v>
+        <v>6532567220.03819</v>
       </c>
       <c r="G11">
         <v>7151.661615179702</v>
@@ -8009,10 +8167,10 @@
         <v>1990</v>
       </c>
       <c r="B12">
-        <v>70.68698450423651</v>
+        <v>70.68698450423649</v>
       </c>
       <c r="C12">
-        <v>4088.264733117415</v>
+        <v>4088.264733117414</v>
       </c>
       <c r="D12">
         <v>10.27536041433178</v>
@@ -8021,10 +8179,10 @@
         <v>1081.759952791378</v>
       </c>
       <c r="F12">
-        <v>6974089587.110185</v>
+        <v>6974089587.110184</v>
       </c>
       <c r="G12">
-        <v>7601.691806306069</v>
+        <v>7601.691806306068</v>
       </c>
       <c r="H12">
         <v>11919632145.40308</v>
@@ -8038,7 +8196,7 @@
         <v>1991</v>
       </c>
       <c r="B13">
-        <v>70.90289896794764</v>
+        <v>70.90289896794765</v>
       </c>
       <c r="C13">
         <v>4140.279252135956</v>
@@ -8073,7 +8231,7 @@
         <v>4195.934359484798</v>
       </c>
       <c r="D14">
-        <v>9.819929690977792</v>
+        <v>9.819929690977791</v>
       </c>
       <c r="E14">
         <v>1224.689758991019</v>
@@ -8102,16 +8260,16 @@
         <v>4253.040708684426</v>
       </c>
       <c r="D15">
-        <v>9.660911117150247</v>
+        <v>9.660911117150246</v>
       </c>
       <c r="E15">
         <v>1345.730479814384</v>
       </c>
       <c r="F15">
-        <v>9256761437.650133</v>
+        <v>9256761437.650131</v>
       </c>
       <c r="G15">
-        <v>9575.006418036213</v>
+        <v>9575.006418036211</v>
       </c>
       <c r="H15">
         <v>15485499581.362</v>
@@ -8125,7 +8283,7 @@
         <v>1994</v>
       </c>
       <c r="B16">
-        <v>71.42972130481625</v>
+        <v>71.42972130481624</v>
       </c>
       <c r="C16">
         <v>4313.781455697557</v>
@@ -8154,7 +8312,7 @@
         <v>1995</v>
       </c>
       <c r="B17">
-        <v>71.57784232783699</v>
+        <v>71.577842327837</v>
       </c>
       <c r="C17">
         <v>4377.51250832132</v>
@@ -8175,7 +8333,7 @@
         <v>18826265019.07761</v>
       </c>
       <c r="I17">
-        <v>23.98506226333385</v>
+        <v>23.98506226333386</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -8186,7 +8344,7 @@
         <v>71.70756403232016</v>
       </c>
       <c r="C18">
-        <v>4447.624094184493</v>
+        <v>4447.624094184494</v>
       </c>
       <c r="D18">
         <v>10.17121900645873</v>
@@ -8212,7 +8370,7 @@
         <v>1997</v>
       </c>
       <c r="B19">
-        <v>71.83182620874901</v>
+        <v>71.83182620874902</v>
       </c>
       <c r="C19">
         <v>4521.231680815152</v>
@@ -8302,7 +8460,7 @@
         <v>72.248065280646</v>
       </c>
       <c r="C22">
-        <v>4740.790142339132</v>
+        <v>4740.790142339131</v>
       </c>
       <c r="D22">
         <v>11.20818970650754</v>
@@ -8317,7 +8475,7 @@
         <v>14649.60562224661</v>
       </c>
       <c r="H22">
-        <v>25963508956.61614</v>
+        <v>25963508956.61613</v>
       </c>
       <c r="I22">
         <v>25.8614860377559</v>
@@ -8328,7 +8486,7 @@
         <v>2001</v>
       </c>
       <c r="B23">
-        <v>72.38106870031348</v>
+        <v>72.38106870031346</v>
       </c>
       <c r="C23">
         <v>4813.147426043226</v>
@@ -8357,10 +8515,10 @@
         <v>2002</v>
       </c>
       <c r="B24">
-        <v>72.50157566822061</v>
+        <v>72.50157566822062</v>
       </c>
       <c r="C24">
-        <v>4879.694917352072</v>
+        <v>4879.694917352071</v>
       </c>
       <c r="D24">
         <v>11.35837618234592</v>
@@ -8386,7 +8544,7 @@
         <v>2003</v>
       </c>
       <c r="B25">
-        <v>72.61659798110347</v>
+        <v>72.61659798110348</v>
       </c>
       <c r="C25">
         <v>4931.479769498702</v>
@@ -8415,7 +8573,7 @@
         <v>2004</v>
       </c>
       <c r="B26">
-        <v>72.73428088092521</v>
+        <v>72.7342808809252</v>
       </c>
       <c r="C26">
         <v>4981.706382863919</v>
@@ -8444,16 +8602,16 @@
         <v>2005</v>
       </c>
       <c r="B27">
-        <v>72.85882900133507</v>
+        <v>72.85882900133505</v>
       </c>
       <c r="C27">
-        <v>5034.304518984587</v>
+        <v>5034.304518984586</v>
       </c>
       <c r="D27">
         <v>12.20563521065967</v>
       </c>
       <c r="E27">
-        <v>3418.291655095759</v>
+        <v>3418.291655095758</v>
       </c>
       <c r="F27">
         <v>19541339702.61924</v>
@@ -8473,7 +8631,7 @@
         <v>2006</v>
       </c>
       <c r="B28">
-        <v>72.99315895796153</v>
+        <v>72.99315895796151</v>
       </c>
       <c r="C28">
         <v>5089.329971837844</v>
@@ -8491,7 +8649,7 @@
         <v>17582.77949495827</v>
       </c>
       <c r="H28">
-        <v>34222901621.69694</v>
+        <v>34222901621.69693</v>
       </c>
       <c r="I28">
         <v>26.57800598580277</v>
@@ -8511,13 +8669,13 @@
         <v>13.34457839297231</v>
       </c>
       <c r="E29">
-        <v>3787.444205784757</v>
+        <v>3787.444205784756</v>
       </c>
       <c r="F29">
         <v>21891468112.40932</v>
       </c>
       <c r="G29">
-        <v>18473.60203886363</v>
+        <v>18473.60203886364</v>
       </c>
       <c r="H29">
         <v>36213813671.78146</v>
@@ -8534,7 +8692,7 @@
         <v>73.30928922305654</v>
       </c>
       <c r="C30">
-        <v>5220.721082191487</v>
+        <v>5220.721082191488</v>
       </c>
       <c r="D30">
         <v>13.09456252940331</v>
@@ -8563,13 +8721,13 @@
         <v>73.49446646576308</v>
       </c>
       <c r="C31">
-        <v>5293.882278321956</v>
+        <v>5293.882278321955</v>
       </c>
       <c r="D31">
         <v>13.05523890016238</v>
       </c>
       <c r="E31">
-        <v>4059.861094844139</v>
+        <v>4059.86109484414</v>
       </c>
       <c r="F31">
         <v>24178087162.88182</v>
@@ -8618,7 +8776,7 @@
         <v>2011</v>
       </c>
       <c r="B33">
-        <v>73.86918409497422</v>
+        <v>73.8691840949742</v>
       </c>
       <c r="C33">
         <v>5438.885047778478</v>
@@ -8636,7 +8794,7 @@
         <v>22285.45380610148</v>
       </c>
       <c r="H33">
-        <v>46468599792.20614</v>
+        <v>46468599792.20615</v>
       </c>
       <c r="I33">
         <v>19.58255150797782</v>
@@ -8647,7 +8805,7 @@
         <v>2012</v>
       </c>
       <c r="B34">
-        <v>74.03115331551265</v>
+        <v>74.03115331551267</v>
       </c>
       <c r="C34">
         <v>5512.77944633687</v>
@@ -8656,7 +8814,7 @@
         <v>13.76375263137036</v>
       </c>
       <c r="E34">
-        <v>4380.429501036875</v>
+        <v>4380.429501036874</v>
       </c>
       <c r="F34">
         <v>28942595521.05588</v>
@@ -8665,7 +8823,7 @@
         <v>23463.79714726256</v>
       </c>
       <c r="H34">
-        <v>49648370340.86935</v>
+        <v>49648370340.86934</v>
       </c>
       <c r="I34">
         <v>19.11682198006619</v>
@@ -8679,7 +8837,7 @@
         <v>74.18101370405006</v>
       </c>
       <c r="C35">
-        <v>5586.158806952898</v>
+        <v>5586.158806952897</v>
       </c>
       <c r="D35">
         <v>14.0114917353758</v>
@@ -8694,7 +8852,7 @@
         <v>24621.30283755035</v>
       </c>
       <c r="H35">
-        <v>52935725627.7122</v>
+        <v>52935725627.71219</v>
       </c>
       <c r="I35">
         <v>17.63840961487545</v>
@@ -8705,7 +8863,7 @@
         <v>2014</v>
       </c>
       <c r="B36">
-        <v>74.32214355880146</v>
+        <v>74.32214355880144</v>
       </c>
       <c r="C36">
         <v>5657.935136284997</v>
@@ -8723,7 +8881,7 @@
         <v>25732.10951147485</v>
       </c>
       <c r="H36">
-        <v>56163572707.60169</v>
+        <v>56163572707.60168</v>
       </c>
       <c r="I36">
         <v>17.99976889212852</v>
@@ -8734,7 +8892,7 @@
         <v>2015</v>
       </c>
       <c r="B37">
-        <v>74.4538519353065</v>
+        <v>74.45385193530649</v>
       </c>
       <c r="C37">
         <v>5728.716801070092</v>
@@ -8752,7 +8910,7 @@
         <v>26717.4788033553</v>
       </c>
       <c r="H37">
-        <v>59117366535.9265</v>
+        <v>59117366535.92649</v>
       </c>
       <c r="I37">
         <v>18.08932985487341</v>
@@ -8763,7 +8921,7 @@
         <v>2016</v>
       </c>
       <c r="B38">
-        <v>74.56618153827139</v>
+        <v>74.56618153827138</v>
       </c>
       <c r="C38">
         <v>5798.914756804919</v>
@@ -8772,7 +8930,7 @@
         <v>14.74237358020609</v>
       </c>
       <c r="E38">
-        <v>4631.799256323041</v>
+        <v>4631.799256323042</v>
       </c>
       <c r="F38">
         <v>34698472064.14433</v>
@@ -8781,7 +8939,7 @@
         <v>27688.10658329666</v>
       </c>
       <c r="H38">
-        <v>62010823638.88225</v>
+        <v>62010823638.88224</v>
       </c>
       <c r="I38">
         <v>17.50825828041602</v>
@@ -8795,22 +8953,22 @@
         <v>74.64939152853269</v>
       </c>
       <c r="C39">
-        <v>5864.546925972781</v>
+        <v>5864.54692597278</v>
       </c>
       <c r="D39">
         <v>15.18861156932739</v>
       </c>
       <c r="E39">
-        <v>4645.382484049745</v>
+        <v>4645.382484049744</v>
       </c>
       <c r="F39">
-        <v>36149218659.08893</v>
+        <v>36149218659.08892</v>
       </c>
       <c r="G39">
         <v>28742.22864924553</v>
       </c>
       <c r="H39">
-        <v>64966169640.30685</v>
+        <v>64966169640.30684</v>
       </c>
       <c r="I39">
         <v>18.58334720710878</v>
@@ -8824,22 +8982,22 @@
         <v>74.69900885124268</v>
       </c>
       <c r="C40">
-        <v>5927.233959463299</v>
+        <v>5927.2339594633</v>
       </c>
       <c r="D40">
         <v>15.38427494968141</v>
       </c>
       <c r="E40">
-        <v>4716.374129679195</v>
+        <v>4716.374129679197</v>
       </c>
       <c r="F40">
         <v>37986013839.80851</v>
       </c>
       <c r="G40">
-        <v>29917.69964302631</v>
+        <v>29917.69964302632</v>
       </c>
       <c r="H40">
-        <v>68125611911.93586</v>
+        <v>68125611911.93587</v>
       </c>
       <c r="I40">
         <v>20.73630601356827</v>
@@ -8850,10 +9008,10 @@
         <v>2019</v>
       </c>
       <c r="B41">
-        <v>74.71642000969267</v>
+        <v>74.71642000969268</v>
       </c>
       <c r="C41">
-        <v>5988.819174167283</v>
+        <v>5988.819174167284</v>
       </c>
       <c r="D41">
         <v>15.81644851756332</v>
@@ -8865,7 +9023,7 @@
         <v>39573043711.04357</v>
       </c>
       <c r="G41">
-        <v>31002.60676855354</v>
+        <v>31002.60676855355</v>
       </c>
       <c r="H41">
         <v>71263689365.37343</v>
@@ -8891,7 +9049,7 @@
         <v>4715.84740302129</v>
       </c>
       <c r="F42">
-        <v>40819182521.63869</v>
+        <v>40819182521.63868</v>
       </c>
       <c r="G42">
         <v>31882.83367939769</v>
@@ -8939,7 +9097,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9000,7 +9158,7 @@
         <v>3242.75390625</v>
       </c>
       <c r="E2">
-        <v>65.44818444609891</v>
+        <v>65.44818444609892</v>
       </c>
       <c r="F2">
         <v>29.76942796998786</v>
@@ -9015,16 +9173,16 @@
         <v>1984168572000</v>
       </c>
       <c r="J2">
-        <v>31459.1389804773</v>
+        <v>31459.13898047731</v>
       </c>
       <c r="K2">
         <v>6757318000000</v>
       </c>
       <c r="L2">
-        <v>25.1299991607666</v>
+        <v>25.12999916076661</v>
       </c>
       <c r="M2">
-        <v>16.08717737576003</v>
+        <v>16.08717737576004</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -9032,7 +9190,7 @@
         <v>1998</v>
       </c>
       <c r="B3">
-        <v>34.65534567454505</v>
+        <v>34.65534567454506</v>
       </c>
       <c r="C3">
         <v>2.492623643269616</v>
@@ -9044,7 +9202,7 @@
         <v>65.53403783771181</v>
       </c>
       <c r="F3">
-        <v>29.95411426532427</v>
+        <v>29.95411426532428</v>
       </c>
       <c r="G3">
         <v>1.903316184460429</v>
@@ -9085,7 +9243,7 @@
         <v>65.62892643128728</v>
       </c>
       <c r="F4">
-        <v>30.14509405403968</v>
+        <v>30.14509405403969</v>
       </c>
       <c r="G4">
         <v>2.403232689272489</v>
@@ -9100,7 +9258,7 @@
         <v>33061.3872343281</v>
       </c>
       <c r="K4">
-        <v>7213220397375.19</v>
+        <v>7213220397375.191</v>
       </c>
       <c r="L4">
         <v>24.89626521651034</v>
@@ -9117,7 +9275,7 @@
         <v>34.4679253969267</v>
       </c>
       <c r="C5">
-        <v>2.54780990456909</v>
+        <v>2.547809904569089</v>
       </c>
       <c r="D5">
         <v>3414.343552384335</v>
@@ -9155,13 +9313,13 @@
         <v>2001</v>
       </c>
       <c r="B6">
-        <v>34.27414573948867</v>
+        <v>34.27414573948866</v>
       </c>
       <c r="C6">
-        <v>2.572841724953723</v>
+        <v>2.572841724953722</v>
       </c>
       <c r="D6">
-        <v>3452.128283106314</v>
+        <v>3452.128283106313</v>
       </c>
       <c r="E6">
         <v>65.83475695503047</v>
@@ -9173,16 +9331,16 @@
         <v>2.432909263264349</v>
       </c>
       <c r="H6">
-        <v>27535.31078591401</v>
+        <v>27535.310785914</v>
       </c>
       <c r="I6">
         <v>2175734577300.279</v>
       </c>
       <c r="J6">
-        <v>34800.40257457241</v>
+        <v>34800.4025745724</v>
       </c>
       <c r="K6">
-        <v>7781463755245.744</v>
+        <v>7781463755245.742</v>
       </c>
       <c r="L6">
         <v>24.50708988812794</v>
@@ -9205,13 +9363,13 @@
         <v>3495.600093562965</v>
       </c>
       <c r="E7">
-        <v>65.93916423451944</v>
+        <v>65.93916423451942</v>
       </c>
       <c r="F7">
         <v>30.71763365330689</v>
       </c>
       <c r="G7">
-        <v>2.123090353723197</v>
+        <v>2.123090353723196</v>
       </c>
       <c r="H7">
         <v>27976.90679329479</v>
@@ -9220,10 +9378,10 @@
         <v>2193534387876.062</v>
       </c>
       <c r="J7">
-        <v>35499.59978688391</v>
+        <v>35499.5997868839</v>
       </c>
       <c r="K7">
-        <v>8046787061366.789</v>
+        <v>8046787061366.788</v>
       </c>
       <c r="L7">
         <v>24.12284993000923</v>
@@ -9237,16 +9395,16 @@
         <v>2003</v>
       </c>
       <c r="B8">
-        <v>33.63011949166695</v>
+        <v>33.63011949166696</v>
       </c>
       <c r="C8">
-        <v>2.568821977105883</v>
+        <v>2.568821977105884</v>
       </c>
       <c r="D8">
-        <v>3573.84104387797</v>
+        <v>3573.841043877971</v>
       </c>
       <c r="E8">
-        <v>66.04074140716793</v>
+        <v>66.04074140716791</v>
       </c>
       <c r="F8">
         <v>30.90440359989413</v>
@@ -9261,10 +9419,10 @@
         <v>2229525730444.568</v>
       </c>
       <c r="J8">
-        <v>36286.7340454277</v>
+        <v>36286.73404542769</v>
       </c>
       <c r="K8">
-        <v>8330884776370.104</v>
+        <v>8330884776370.103</v>
       </c>
       <c r="L8">
         <v>23.79289150616501</v>
@@ -9287,7 +9445,7 @@
         <v>3612.427475837603</v>
       </c>
       <c r="E9">
-        <v>66.14537607160986</v>
+        <v>66.14537607160985</v>
       </c>
       <c r="F9">
         <v>31.09571432879839</v>
@@ -9325,10 +9483,10 @@
         <v>2.550037054569662</v>
       </c>
       <c r="D10">
-        <v>3633.983746483734</v>
+        <v>3633.983746483735</v>
       </c>
       <c r="E10">
-        <v>66.25743074739589</v>
+        <v>66.2574307473959</v>
       </c>
       <c r="F10">
         <v>31.29198787067715</v>
@@ -9343,10 +9501,10 @@
         <v>2369943238852.363</v>
       </c>
       <c r="J10">
-        <v>38433.14819287535</v>
+        <v>38433.14819287536</v>
       </c>
       <c r="K10">
-        <v>9001469600847.461</v>
+        <v>9001469600847.463</v>
       </c>
       <c r="L10">
         <v>23.32192376253722</v>
@@ -9369,7 +9527,7 @@
         <v>3660.978677260224</v>
       </c>
       <c r="E11">
-        <v>66.3444044933793</v>
+        <v>66.34440449337932</v>
       </c>
       <c r="F11">
         <v>31.49585131681092</v>
@@ -9381,16 +9539,16 @@
         <v>33115.57612637409</v>
       </c>
       <c r="I11">
-        <v>2467833575413.643</v>
+        <v>2467833575413.644</v>
       </c>
       <c r="J11">
         <v>39690.91545282934</v>
       </c>
       <c r="K11">
-        <v>9376891848604.68</v>
+        <v>9376891848604.682</v>
       </c>
       <c r="L11">
-        <v>23.16657031312142</v>
+        <v>23.16657031312143</v>
       </c>
       <c r="M11">
         <v>12.99072266531401</v>
@@ -9410,7 +9568,7 @@
         <v>3678.721528749189</v>
       </c>
       <c r="E12">
-        <v>66.41958988015294</v>
+        <v>66.41958988015293</v>
       </c>
       <c r="F12">
         <v>31.70638038056141</v>
@@ -9422,13 +9580,13 @@
         <v>34257.80129595214</v>
       </c>
       <c r="I12">
-        <v>2564225990312.376</v>
+        <v>2564225990312.375</v>
       </c>
       <c r="J12">
-        <v>40963.64340196887</v>
+        <v>40963.64340196886</v>
       </c>
       <c r="K12">
-        <v>9767912643341.949</v>
+        <v>9767912643341.947</v>
       </c>
       <c r="L12">
         <v>23.01027203395847</v>
@@ -9463,7 +9621,7 @@
         <v>34996.35419099942</v>
       </c>
       <c r="I13">
-        <v>2638280830462.706</v>
+        <v>2638280830462.707</v>
       </c>
       <c r="J13">
         <v>42074.79030845637</v>
@@ -9513,7 +9671,7 @@
         <v>10459122417681.08</v>
       </c>
       <c r="L14">
-        <v>22.39130903995167</v>
+        <v>22.39130903995166</v>
       </c>
       <c r="M14">
         <v>11.69878959461227</v>
@@ -9524,7 +9682,7 @@
         <v>2010</v>
       </c>
       <c r="B15">
-        <v>32.02622352541319</v>
+        <v>32.02622352541318</v>
       </c>
       <c r="C15">
         <v>2.639472932147355</v>
@@ -9533,7 +9691,7 @@
         <v>3784.13662059177</v>
       </c>
       <c r="E15">
-        <v>66.579131463758</v>
+        <v>66.57913146375799</v>
       </c>
       <c r="F15">
         <v>32.38411249865136</v>
@@ -9548,7 +9706,7 @@
         <v>2693321704950.166</v>
       </c>
       <c r="J15">
-        <v>43597.25346685877</v>
+        <v>43597.25346685876</v>
       </c>
       <c r="K15">
         <v>10775324244543.01</v>
@@ -9583,7 +9741,7 @@
         <v>1.809897178766296</v>
       </c>
       <c r="H16">
-        <v>36139.59617541145</v>
+        <v>36139.59617541144</v>
       </c>
       <c r="I16">
         <v>2737833709460.516</v>
@@ -9606,16 +9764,16 @@
         <v>2012</v>
       </c>
       <c r="B17">
-        <v>31.32164383484101</v>
+        <v>31.32164383484102</v>
       </c>
       <c r="C17">
         <v>2.659536229789733</v>
       </c>
       <c r="D17">
-        <v>3838.828561173246</v>
+        <v>3838.828561173247</v>
       </c>
       <c r="E17">
-        <v>66.60070597024213</v>
+        <v>66.60070597024215</v>
       </c>
       <c r="F17">
         <v>32.82967302099993</v>
@@ -9627,10 +9785,10 @@
         <v>36526.43548679419</v>
       </c>
       <c r="I17">
-        <v>2786889444319.623</v>
+        <v>2786889444319.624</v>
       </c>
       <c r="J17">
-        <v>45412.4201391015</v>
+        <v>45412.42013910151</v>
       </c>
       <c r="K17">
         <v>11420262453385.14</v>
@@ -9647,7 +9805,7 @@
         <v>2013</v>
       </c>
       <c r="B18">
-        <v>31.08410075458201</v>
+        <v>31.08410075458202</v>
       </c>
       <c r="C18">
         <v>2.6661718308614</v>
@@ -9659,13 +9817,13 @@
         <v>66.58503698957099</v>
       </c>
       <c r="F18">
-        <v>33.04941552559389</v>
+        <v>33.0494155255939</v>
       </c>
       <c r="G18">
         <v>1.766609016152382</v>
       </c>
       <c r="H18">
-        <v>36601.35155720384</v>
+        <v>36601.35155720385</v>
       </c>
       <c r="I18">
         <v>2844820998391.466</v>
@@ -9674,7 +9832,7 @@
         <v>46417.73141534033</v>
       </c>
       <c r="K18">
-        <v>11736184928697.51</v>
+        <v>11736184928697.52</v>
       </c>
       <c r="L18">
         <v>21.26022141934975</v>
@@ -9738,7 +9896,7 @@
         <v>3957.059324545885</v>
       </c>
       <c r="E20">
-        <v>66.4996997857707</v>
+        <v>66.49969978577069</v>
       </c>
       <c r="F20">
         <v>33.49119150814992</v>
@@ -9753,7 +9911,7 @@
         <v>2971630058900.723</v>
       </c>
       <c r="J20">
-        <v>48652.10964751362</v>
+        <v>48652.10964751363</v>
       </c>
       <c r="K20">
         <v>12417795084835.92</v>
@@ -9782,16 +9940,16 @@
         <v>66.43186488913413</v>
       </c>
       <c r="F21">
-        <v>33.71382530406733</v>
+        <v>33.71382530406732</v>
       </c>
       <c r="G21">
         <v>1.941593459873912</v>
       </c>
       <c r="H21">
-        <v>37145.83206137943</v>
+        <v>37145.83206137942</v>
       </c>
       <c r="I21">
-        <v>3020537478528.385</v>
+        <v>3020537478528.384</v>
       </c>
       <c r="J21">
         <v>49774.88714688006</v>
@@ -9814,34 +9972,34 @@
         <v>30.33105977641117</v>
       </c>
       <c r="C22">
-        <v>2.728822830641545</v>
+        <v>2.728822830641546</v>
       </c>
       <c r="D22">
-        <v>4043.327778947728</v>
+        <v>4043.327778947729</v>
       </c>
       <c r="E22">
-        <v>66.34639533405544</v>
+        <v>66.34639533405546</v>
       </c>
       <c r="F22">
-        <v>33.93403469839269</v>
+        <v>33.9340346983927</v>
       </c>
       <c r="G22">
-        <v>1.943205674622268</v>
+        <v>1.943205674622269</v>
       </c>
       <c r="H22">
         <v>37681.18808564563</v>
       </c>
       <c r="I22">
-        <v>3089278640374.658</v>
+        <v>3089278640374.659</v>
       </c>
       <c r="J22">
-        <v>50995.938383661</v>
+        <v>50995.93838366101</v>
       </c>
       <c r="K22">
         <v>13160469714997.85</v>
       </c>
       <c r="L22">
-        <v>20.67506785225224</v>
+        <v>20.67506785225225</v>
       </c>
       <c r="M22">
         <v>11.25487168998816</v>
@@ -9852,10 +10010,10 @@
         <v>2018</v>
       </c>
       <c r="B23">
-        <v>30.21533026041826</v>
+        <v>30.21533026041827</v>
       </c>
       <c r="C23">
-        <v>2.761239075476049</v>
+        <v>2.76123907547605</v>
       </c>
       <c r="D23">
         <v>4127.409983899511</v>
@@ -9870,19 +10028,19 @@
         <v>1.836278468076208</v>
       </c>
       <c r="H23">
-        <v>38313.32491038368</v>
+        <v>38313.32491038369</v>
       </c>
       <c r="I23">
         <v>3176543168615.03</v>
       </c>
       <c r="J23">
-        <v>52403.35659281567</v>
+        <v>52403.35659281568</v>
       </c>
       <c r="K23">
         <v>13592191769915.74</v>
       </c>
       <c r="L23">
-        <v>20.57912105620212</v>
+        <v>20.57912105620213</v>
       </c>
       <c r="M23">
         <v>11.34219756039769</v>
@@ -9911,13 +10069,13 @@
         <v>1.793336323342798</v>
       </c>
       <c r="H24">
-        <v>38807.54386211564</v>
+        <v>38807.54386211565</v>
       </c>
       <c r="I24">
-        <v>3263188992652.463</v>
+        <v>3263188992652.462</v>
       </c>
       <c r="J24">
-        <v>53902.14867686526</v>
+        <v>53902.14867686527</v>
       </c>
       <c r="K24">
         <v>14042180063075.43</v>
@@ -9968,6 +10126,47 @@
       </c>
       <c r="M25">
         <v>11.18777772755131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>2021</v>
+      </c>
+      <c r="B26">
+        <v>30.34971078112964</v>
+      </c>
+      <c r="C26">
+        <v>3.000267417503025</v>
+      </c>
+      <c r="D26">
+        <v>4039.521382983692</v>
+      </c>
+      <c r="E26">
+        <v>65.84887099317973</v>
+      </c>
+      <c r="F26">
+        <v>34.84003218292119</v>
+      </c>
+      <c r="G26">
+        <v>1.207045785819274</v>
+      </c>
+      <c r="H26">
+        <v>38908.74612618054</v>
+      </c>
+      <c r="I26">
+        <v>3367852388831.007</v>
+      </c>
+      <c r="J26">
+        <v>54986.67619464755</v>
+      </c>
+      <c r="K26">
+        <v>14551440506422.67</v>
+      </c>
+      <c r="L26">
+        <v>20.66534582190606</v>
+      </c>
+      <c r="M26">
+        <v>12.71094963783942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>